<commit_message>
author-info complete and ready for final checks
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="91">
   <si>
     <t>SITES</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>85.375em</t>
-  </si>
-  <si>
-    <t>Font Resposiveness</t>
   </si>
 </sst>
 </file>
@@ -670,7 +667,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="138">
+  <cellStyleXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -809,8 +806,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -967,6 +972,15 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -998,6 +1012,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1037,9 +1054,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1138,9 +1152,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1160,7 +1171,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="138">
+  <cellStyles count="146">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1229,6 +1240,10 @@
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1297,10 +1312,164 @@
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="209">
+  <dxfs count="224">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3722,8 +3891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63:E64"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3734,36 +3903,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="25" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="67" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="81"/>
+      <c r="X1" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="69"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="73"/>
       <c r="AA1" s="36"/>
       <c r="AB1" s="36"/>
       <c r="AC1" s="36"/>
@@ -3777,34 +3946,34 @@
       <c r="AK1" s="36"/>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="77"/>
-      <c r="X2" s="70" t="s">
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="72"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="76"/>
       <c r="AA2" s="36"/>
       <c r="AB2" s="36"/>
       <c r="AC2" s="36"/>
@@ -3818,34 +3987,34 @@
       <c r="AK2" s="36"/>
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1">
-      <c r="A3" s="76"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="70" t="s">
+      <c r="A3" s="80"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="81"/>
+      <c r="X3" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="Y3" s="71"/>
-      <c r="Z3" s="72"/>
+      <c r="Y3" s="75"/>
+      <c r="Z3" s="76"/>
       <c r="AA3" s="36"/>
       <c r="AB3" s="36"/>
       <c r="AC3" s="36"/>
@@ -3859,34 +4028,34 @@
       <c r="AK3" s="36"/>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1">
-      <c r="A4" s="76"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="76"/>
-      <c r="S4" s="76"/>
-      <c r="T4" s="76"/>
-      <c r="U4" s="76"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="70" t="s">
+      <c r="A4" s="80"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="Y4" s="71"/>
-      <c r="Z4" s="72"/>
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="76"/>
       <c r="AA4" s="36"/>
       <c r="AB4" s="36"/>
       <c r="AC4" s="36"/>
@@ -3900,34 +4069,34 @@
       <c r="AK4" s="36"/>
     </row>
     <row r="5" spans="1:37" ht="16" customHeight="1" thickBot="1">
-      <c r="A5" s="76"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="76"/>
-      <c r="S5" s="76"/>
-      <c r="T5" s="76"/>
-      <c r="U5" s="76"/>
-      <c r="V5" s="76"/>
-      <c r="W5" s="77"/>
-      <c r="X5" s="73" t="s">
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="Y5" s="74"/>
-      <c r="Z5" s="75"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="79"/>
       <c r="AA5" s="36"/>
       <c r="AB5" s="36"/>
       <c r="AC5" s="36"/>
@@ -3941,31 +4110,31 @@
       <c r="AK5" s="36"/>
     </row>
     <row r="6" spans="1:37" ht="16" thickBot="1">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
-      <c r="X6" s="78"/>
-      <c r="Y6" s="78"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="82"/>
+      <c r="Y6" s="82"/>
       <c r="Z6" s="41"/>
       <c r="AA6" s="36"/>
       <c r="AB6" s="36"/>
@@ -3980,46 +4149,46 @@
       <c r="AK6" s="36"/>
     </row>
     <row r="7" spans="1:37">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="79" t="s">
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="115"/>
-      <c r="J7" s="79" t="s">
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="114"/>
-      <c r="L7" s="114"/>
-      <c r="M7" s="115"/>
-      <c r="N7" s="79" t="s">
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
+      <c r="M7" s="117"/>
+      <c r="N7" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="114"/>
-      <c r="P7" s="114"/>
-      <c r="Q7" s="115"/>
-      <c r="R7" s="79" t="s">
+      <c r="O7" s="116"/>
+      <c r="P7" s="116"/>
+      <c r="Q7" s="117"/>
+      <c r="R7" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="114"/>
-      <c r="T7" s="114"/>
-      <c r="U7" s="115"/>
-      <c r="V7" s="114" t="s">
+      <c r="S7" s="116"/>
+      <c r="T7" s="116"/>
+      <c r="U7" s="117"/>
+      <c r="V7" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="W7" s="114"/>
-      <c r="X7" s="114"/>
-      <c r="Y7" s="114"/>
-      <c r="Z7" s="92" t="s">
+      <c r="W7" s="116"/>
+      <c r="X7" s="116"/>
+      <c r="Y7" s="116"/>
+      <c r="Z7" s="95" t="s">
         <v>53</v>
       </c>
       <c r="AA7" s="36"/>
@@ -4035,32 +4204,32 @@
       <c r="AK7" s="36"/>
     </row>
     <row r="8" spans="1:37">
-      <c r="A8" s="85"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="117"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="117"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="116"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="117"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="116"/>
-      <c r="T8" s="116"/>
-      <c r="U8" s="117"/>
-      <c r="V8" s="116"/>
-      <c r="W8" s="116"/>
-      <c r="X8" s="116"/>
-      <c r="Y8" s="116"/>
-      <c r="Z8" s="93"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="118"/>
+      <c r="P8" s="118"/>
+      <c r="Q8" s="119"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="118"/>
+      <c r="T8" s="118"/>
+      <c r="U8" s="119"/>
+      <c r="V8" s="118"/>
+      <c r="W8" s="118"/>
+      <c r="X8" s="118"/>
+      <c r="Y8" s="118"/>
+      <c r="Z8" s="96"/>
       <c r="AA8" s="36"/>
       <c r="AB8" s="36"/>
       <c r="AC8" s="36"/>
@@ -4074,7 +4243,7 @@
       <c r="AK8" s="36"/>
     </row>
     <row r="9" spans="1:37" ht="16" thickBot="1">
-      <c r="A9" s="86"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="44" t="s">
         <v>25</v>
       </c>
@@ -4147,7 +4316,7 @@
       <c r="Y9" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Z9" s="94"/>
+      <c r="Z9" s="97"/>
       <c r="AA9" s="36"/>
       <c r="AB9" s="36"/>
       <c r="AC9" s="36"/>
@@ -4161,7 +4330,7 @@
       <c r="AK9" s="36"/>
     </row>
     <row r="10" spans="1:37">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="90" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -4236,7 +4405,7 @@
       <c r="Y10" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="Z10" s="95" t="s">
+      <c r="Z10" s="98" t="s">
         <v>50</v>
       </c>
       <c r="AA10" s="36"/>
@@ -4252,44 +4421,44 @@
       <c r="AK10" s="36"/>
     </row>
     <row r="11" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A11" s="88"/>
-      <c r="B11" s="89" t="s">
+      <c r="A11" s="91"/>
+      <c r="B11" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="89" t="s">
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="89" t="s">
+      <c r="G11" s="93"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="91"/>
-      <c r="N11" s="98" t="s">
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="94"/>
+      <c r="N11" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="99"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="100"/>
-      <c r="R11" s="89" t="s">
+      <c r="O11" s="102"/>
+      <c r="P11" s="102"/>
+      <c r="Q11" s="103"/>
+      <c r="R11" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="91"/>
-      <c r="V11" s="89" t="s">
+      <c r="S11" s="93"/>
+      <c r="T11" s="93"/>
+      <c r="U11" s="94"/>
+      <c r="V11" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W11" s="90"/>
-      <c r="X11" s="90"/>
-      <c r="Y11" s="91"/>
-      <c r="Z11" s="97"/>
+      <c r="W11" s="93"/>
+      <c r="X11" s="93"/>
+      <c r="Y11" s="94"/>
+      <c r="Z11" s="100"/>
       <c r="AA11" s="53"/>
       <c r="AB11" s="53"/>
       <c r="AC11" s="53"/>
@@ -4303,7 +4472,7 @@
       <c r="AK11" s="53"/>
     </row>
     <row r="12" spans="1:37">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="90" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -4378,7 +4547,7 @@
       <c r="Y12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z12" s="58" t="s">
+      <c r="Z12" s="61" t="s">
         <v>50</v>
       </c>
       <c r="AA12" s="36"/>
@@ -4394,44 +4563,44 @@
       <c r="AK12" s="36"/>
     </row>
     <row r="13" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A13" s="88"/>
-      <c r="B13" s="89" t="s">
+      <c r="A13" s="91"/>
+      <c r="B13" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="89" t="s">
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="89" t="s">
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="91"/>
-      <c r="N13" s="98" t="s">
+      <c r="K13" s="93"/>
+      <c r="L13" s="93"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O13" s="99"/>
-      <c r="P13" s="99"/>
-      <c r="Q13" s="100"/>
-      <c r="R13" s="89" t="s">
+      <c r="O13" s="102"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="91"/>
-      <c r="V13" s="89" t="s">
+      <c r="S13" s="93"/>
+      <c r="T13" s="93"/>
+      <c r="U13" s="94"/>
+      <c r="V13" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W13" s="90"/>
-      <c r="X13" s="90"/>
-      <c r="Y13" s="91"/>
-      <c r="Z13" s="61"/>
+      <c r="W13" s="93"/>
+      <c r="X13" s="93"/>
+      <c r="Y13" s="94"/>
+      <c r="Z13" s="64"/>
       <c r="AA13" s="53"/>
       <c r="AB13" s="53"/>
       <c r="AC13" s="53"/>
@@ -4445,7 +4614,7 @@
       <c r="AK13" s="53"/>
     </row>
     <row r="14" spans="1:37">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="90" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="15" t="s">
@@ -4520,7 +4689,7 @@
       <c r="Y14" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z14" s="58" t="s">
+      <c r="Z14" s="61" t="s">
         <v>50</v>
       </c>
       <c r="AA14" s="54"/>
@@ -4536,44 +4705,44 @@
       <c r="AK14" s="36"/>
     </row>
     <row r="15" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A15" s="88"/>
-      <c r="B15" s="89" t="s">
+      <c r="A15" s="91"/>
+      <c r="B15" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="89" t="s">
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="89" t="s">
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="98" t="s">
+      <c r="K15" s="93"/>
+      <c r="L15" s="93"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O15" s="99"/>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="100"/>
-      <c r="R15" s="89" t="s">
+      <c r="O15" s="102"/>
+      <c r="P15" s="102"/>
+      <c r="Q15" s="103"/>
+      <c r="R15" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
-      <c r="U15" s="91"/>
-      <c r="V15" s="89" t="s">
+      <c r="S15" s="93"/>
+      <c r="T15" s="93"/>
+      <c r="U15" s="94"/>
+      <c r="V15" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W15" s="90"/>
-      <c r="X15" s="90"/>
-      <c r="Y15" s="91"/>
-      <c r="Z15" s="61"/>
+      <c r="W15" s="93"/>
+      <c r="X15" s="93"/>
+      <c r="Y15" s="94"/>
+      <c r="Z15" s="64"/>
       <c r="AA15" s="55"/>
       <c r="AB15" s="53"/>
       <c r="AC15" s="53"/>
@@ -4587,7 +4756,7 @@
       <c r="AK15" s="53"/>
     </row>
     <row r="16" spans="1:37">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="90" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="15" t="s">
@@ -4662,7 +4831,7 @@
       <c r="Y16" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z16" s="58" t="s">
+      <c r="Z16" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA16" s="36"/>
@@ -4678,44 +4847,44 @@
       <c r="AK16" s="36"/>
     </row>
     <row r="17" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A17" s="88"/>
-      <c r="B17" s="89" t="s">
+      <c r="A17" s="91"/>
+      <c r="B17" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="89" t="s">
+      <c r="C17" s="93"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="89" t="s">
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="90"/>
-      <c r="L17" s="90"/>
-      <c r="M17" s="91"/>
-      <c r="N17" s="98" t="s">
+      <c r="K17" s="93"/>
+      <c r="L17" s="93"/>
+      <c r="M17" s="94"/>
+      <c r="N17" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="99"/>
-      <c r="P17" s="99"/>
-      <c r="Q17" s="100"/>
-      <c r="R17" s="89" t="s">
+      <c r="O17" s="102"/>
+      <c r="P17" s="102"/>
+      <c r="Q17" s="103"/>
+      <c r="R17" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S17" s="90"/>
-      <c r="T17" s="90"/>
-      <c r="U17" s="91"/>
-      <c r="V17" s="89" t="s">
+      <c r="S17" s="93"/>
+      <c r="T17" s="93"/>
+      <c r="U17" s="94"/>
+      <c r="V17" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W17" s="90"/>
-      <c r="X17" s="90"/>
-      <c r="Y17" s="91"/>
-      <c r="Z17" s="61"/>
+      <c r="W17" s="93"/>
+      <c r="X17" s="93"/>
+      <c r="Y17" s="94"/>
+      <c r="Z17" s="64"/>
       <c r="AA17" s="53"/>
       <c r="AB17" s="53"/>
       <c r="AC17" s="53"/>
@@ -4729,7 +4898,7 @@
       <c r="AK17" s="53"/>
     </row>
     <row r="18" spans="1:37">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="90" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="15" t="s">
@@ -4804,7 +4973,7 @@
       <c r="Y18" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z18" s="58" t="s">
+      <c r="Z18" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA18" s="36"/>
@@ -4820,44 +4989,44 @@
       <c r="AK18" s="36"/>
     </row>
     <row r="19" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A19" s="88"/>
-      <c r="B19" s="89" t="s">
+      <c r="A19" s="91"/>
+      <c r="B19" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="89" t="s">
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="89" t="s">
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K19" s="90"/>
-      <c r="L19" s="90"/>
-      <c r="M19" s="91"/>
-      <c r="N19" s="98" t="s">
+      <c r="K19" s="93"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="94"/>
+      <c r="N19" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O19" s="99"/>
-      <c r="P19" s="99"/>
-      <c r="Q19" s="100"/>
-      <c r="R19" s="89" t="s">
+      <c r="O19" s="102"/>
+      <c r="P19" s="102"/>
+      <c r="Q19" s="103"/>
+      <c r="R19" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S19" s="90"/>
-      <c r="T19" s="90"/>
-      <c r="U19" s="91"/>
-      <c r="V19" s="89" t="s">
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="94"/>
+      <c r="V19" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W19" s="90"/>
-      <c r="X19" s="90"/>
-      <c r="Y19" s="91"/>
-      <c r="Z19" s="61"/>
+      <c r="W19" s="93"/>
+      <c r="X19" s="93"/>
+      <c r="Y19" s="94"/>
+      <c r="Z19" s="64"/>
       <c r="AA19" s="53"/>
       <c r="AB19" s="53"/>
       <c r="AC19" s="53"/>
@@ -4871,7 +5040,7 @@
       <c r="AK19" s="53"/>
     </row>
     <row r="20" spans="1:37">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="90" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="15" t="s">
@@ -4946,7 +5115,7 @@
       <c r="Y20" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z20" s="58" t="s">
+      <c r="Z20" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA20" s="36"/>
@@ -4962,44 +5131,44 @@
       <c r="AK20" s="36"/>
     </row>
     <row r="21" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A21" s="88"/>
-      <c r="B21" s="89" t="s">
+      <c r="A21" s="91"/>
+      <c r="B21" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="90"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="89" t="s">
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="90"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="91"/>
-      <c r="J21" s="89" t="s">
+      <c r="G21" s="93"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K21" s="90"/>
-      <c r="L21" s="90"/>
-      <c r="M21" s="91"/>
-      <c r="N21" s="98" t="s">
+      <c r="K21" s="93"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="94"/>
+      <c r="N21" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O21" s="99"/>
-      <c r="P21" s="99"/>
-      <c r="Q21" s="100"/>
-      <c r="R21" s="89" t="s">
+      <c r="O21" s="102"/>
+      <c r="P21" s="102"/>
+      <c r="Q21" s="103"/>
+      <c r="R21" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S21" s="90"/>
-      <c r="T21" s="90"/>
-      <c r="U21" s="91"/>
-      <c r="V21" s="89" t="s">
+      <c r="S21" s="93"/>
+      <c r="T21" s="93"/>
+      <c r="U21" s="94"/>
+      <c r="V21" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W21" s="90"/>
-      <c r="X21" s="90"/>
-      <c r="Y21" s="91"/>
-      <c r="Z21" s="61"/>
+      <c r="W21" s="93"/>
+      <c r="X21" s="93"/>
+      <c r="Y21" s="94"/>
+      <c r="Z21" s="64"/>
       <c r="AA21" s="53"/>
       <c r="AB21" s="53"/>
       <c r="AC21" s="53"/>
@@ -5013,7 +5182,7 @@
       <c r="AK21" s="53"/>
     </row>
     <row r="22" spans="1:37">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="90" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -5088,7 +5257,7 @@
       <c r="Y22" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z22" s="58" t="s">
+      <c r="Z22" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA22" s="36"/>
@@ -5104,44 +5273,44 @@
       <c r="AK22" s="36"/>
     </row>
     <row r="23" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A23" s="88"/>
-      <c r="B23" s="89" t="s">
+      <c r="A23" s="91"/>
+      <c r="B23" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="90"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="89" t="s">
+      <c r="C23" s="93"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="90"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="89" t="s">
+      <c r="G23" s="93"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="94"/>
+      <c r="J23" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K23" s="90"/>
-      <c r="L23" s="90"/>
-      <c r="M23" s="91"/>
-      <c r="N23" s="98" t="s">
+      <c r="K23" s="93"/>
+      <c r="L23" s="93"/>
+      <c r="M23" s="94"/>
+      <c r="N23" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O23" s="99"/>
-      <c r="P23" s="99"/>
-      <c r="Q23" s="100"/>
-      <c r="R23" s="89" t="s">
+      <c r="O23" s="102"/>
+      <c r="P23" s="102"/>
+      <c r="Q23" s="103"/>
+      <c r="R23" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S23" s="90"/>
-      <c r="T23" s="90"/>
-      <c r="U23" s="91"/>
-      <c r="V23" s="89" t="s">
+      <c r="S23" s="93"/>
+      <c r="T23" s="93"/>
+      <c r="U23" s="94"/>
+      <c r="V23" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W23" s="90"/>
-      <c r="X23" s="90"/>
-      <c r="Y23" s="91"/>
-      <c r="Z23" s="61"/>
+      <c r="W23" s="93"/>
+      <c r="X23" s="93"/>
+      <c r="Y23" s="94"/>
+      <c r="Z23" s="64"/>
       <c r="AA23" s="53"/>
       <c r="AB23" s="53"/>
       <c r="AC23" s="53"/>
@@ -5155,7 +5324,7 @@
       <c r="AK23" s="53"/>
     </row>
     <row r="24" spans="1:37">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="90" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="15" t="s">
@@ -5230,7 +5399,7 @@
       <c r="Y24" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z24" s="58" t="s">
+      <c r="Z24" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA24" s="36"/>
@@ -5246,44 +5415,44 @@
       <c r="AK24" s="36"/>
     </row>
     <row r="25" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A25" s="88"/>
-      <c r="B25" s="89" t="s">
+      <c r="A25" s="91"/>
+      <c r="B25" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="89" t="s">
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="89" t="s">
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="94"/>
+      <c r="J25" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="91"/>
-      <c r="N25" s="98" t="s">
+      <c r="K25" s="93"/>
+      <c r="L25" s="93"/>
+      <c r="M25" s="94"/>
+      <c r="N25" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O25" s="99"/>
-      <c r="P25" s="99"/>
-      <c r="Q25" s="100"/>
-      <c r="R25" s="89" t="s">
+      <c r="O25" s="102"/>
+      <c r="P25" s="102"/>
+      <c r="Q25" s="103"/>
+      <c r="R25" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S25" s="90"/>
-      <c r="T25" s="90"/>
-      <c r="U25" s="91"/>
-      <c r="V25" s="89" t="s">
+      <c r="S25" s="93"/>
+      <c r="T25" s="93"/>
+      <c r="U25" s="94"/>
+      <c r="V25" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W25" s="90"/>
-      <c r="X25" s="90"/>
-      <c r="Y25" s="91"/>
-      <c r="Z25" s="61"/>
+      <c r="W25" s="93"/>
+      <c r="X25" s="93"/>
+      <c r="Y25" s="94"/>
+      <c r="Z25" s="64"/>
       <c r="AA25" s="53"/>
       <c r="AB25" s="53"/>
       <c r="AC25" s="53"/>
@@ -5297,7 +5466,7 @@
       <c r="AK25" s="53"/>
     </row>
     <row r="26" spans="1:37">
-      <c r="A26" s="87" t="s">
+      <c r="A26" s="90" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="15" t="s">
@@ -5372,7 +5541,7 @@
       <c r="Y26" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z26" s="58" t="s">
+      <c r="Z26" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA26" s="36"/>
@@ -5388,44 +5557,44 @@
       <c r="AK26" s="36"/>
     </row>
     <row r="27" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A27" s="88"/>
-      <c r="B27" s="89" t="s">
+      <c r="A27" s="91"/>
+      <c r="B27" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="90"/>
-      <c r="D27" s="90"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="89" t="s">
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="94"/>
+      <c r="F27" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="89" t="s">
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="94"/>
+      <c r="J27" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="91"/>
-      <c r="N27" s="98" t="s">
+      <c r="K27" s="93"/>
+      <c r="L27" s="93"/>
+      <c r="M27" s="94"/>
+      <c r="N27" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O27" s="99"/>
-      <c r="P27" s="99"/>
-      <c r="Q27" s="100"/>
-      <c r="R27" s="89" t="s">
+      <c r="O27" s="102"/>
+      <c r="P27" s="102"/>
+      <c r="Q27" s="103"/>
+      <c r="R27" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S27" s="90"/>
-      <c r="T27" s="90"/>
-      <c r="U27" s="91"/>
-      <c r="V27" s="89" t="s">
+      <c r="S27" s="93"/>
+      <c r="T27" s="93"/>
+      <c r="U27" s="94"/>
+      <c r="V27" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W27" s="90"/>
-      <c r="X27" s="90"/>
-      <c r="Y27" s="91"/>
-      <c r="Z27" s="61"/>
+      <c r="W27" s="93"/>
+      <c r="X27" s="93"/>
+      <c r="Y27" s="94"/>
+      <c r="Z27" s="64"/>
       <c r="AA27" s="53"/>
       <c r="AB27" s="53"/>
       <c r="AC27" s="53"/>
@@ -5439,7 +5608,7 @@
       <c r="AK27" s="53"/>
     </row>
     <row r="28" spans="1:37">
-      <c r="A28" s="87" t="s">
+      <c r="A28" s="90" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5514,7 +5683,7 @@
       <c r="Y28" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z28" s="58" t="s">
+      <c r="Z28" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA28" s="36"/>
@@ -5530,44 +5699,44 @@
       <c r="AK28" s="36"/>
     </row>
     <row r="29" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A29" s="88"/>
-      <c r="B29" s="89" t="s">
+      <c r="A29" s="91"/>
+      <c r="B29" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="89" t="s">
+      <c r="C29" s="93"/>
+      <c r="D29" s="93"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="89" t="s">
+      <c r="G29" s="93"/>
+      <c r="H29" s="93"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="91"/>
-      <c r="N29" s="98" t="s">
+      <c r="K29" s="93"/>
+      <c r="L29" s="93"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O29" s="99"/>
-      <c r="P29" s="99"/>
-      <c r="Q29" s="100"/>
-      <c r="R29" s="89" t="s">
+      <c r="O29" s="102"/>
+      <c r="P29" s="102"/>
+      <c r="Q29" s="103"/>
+      <c r="R29" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S29" s="90"/>
-      <c r="T29" s="90"/>
-      <c r="U29" s="91"/>
-      <c r="V29" s="89" t="s">
+      <c r="S29" s="93"/>
+      <c r="T29" s="93"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W29" s="90"/>
-      <c r="X29" s="90"/>
-      <c r="Y29" s="91"/>
-      <c r="Z29" s="61"/>
+      <c r="W29" s="93"/>
+      <c r="X29" s="93"/>
+      <c r="Y29" s="94"/>
+      <c r="Z29" s="64"/>
       <c r="AA29" s="53"/>
       <c r="AB29" s="53"/>
       <c r="AC29" s="53"/>
@@ -5581,7 +5750,7 @@
       <c r="AK29" s="53"/>
     </row>
     <row r="30" spans="1:37">
-      <c r="A30" s="87" t="s">
+      <c r="A30" s="90" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -5656,7 +5825,7 @@
       <c r="Y30" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z30" s="58" t="s">
+      <c r="Z30" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA30" s="36"/>
@@ -5672,44 +5841,44 @@
       <c r="AK30" s="36"/>
     </row>
     <row r="31" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A31" s="88"/>
-      <c r="B31" s="89" t="s">
+      <c r="A31" s="91"/>
+      <c r="B31" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="89" t="s">
+      <c r="C31" s="93"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G31" s="90"/>
-      <c r="H31" s="90"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="89" t="s">
+      <c r="G31" s="93"/>
+      <c r="H31" s="93"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K31" s="90"/>
-      <c r="L31" s="90"/>
-      <c r="M31" s="91"/>
-      <c r="N31" s="98" t="s">
+      <c r="K31" s="93"/>
+      <c r="L31" s="93"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="100"/>
-      <c r="R31" s="89" t="s">
+      <c r="O31" s="102"/>
+      <c r="P31" s="102"/>
+      <c r="Q31" s="103"/>
+      <c r="R31" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S31" s="90"/>
-      <c r="T31" s="90"/>
-      <c r="U31" s="91"/>
-      <c r="V31" s="89" t="s">
+      <c r="S31" s="93"/>
+      <c r="T31" s="93"/>
+      <c r="U31" s="94"/>
+      <c r="V31" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W31" s="90"/>
-      <c r="X31" s="90"/>
-      <c r="Y31" s="91"/>
-      <c r="Z31" s="61"/>
+      <c r="W31" s="93"/>
+      <c r="X31" s="93"/>
+      <c r="Y31" s="94"/>
+      <c r="Z31" s="64"/>
       <c r="AA31" s="53"/>
       <c r="AB31" s="53"/>
       <c r="AC31" s="53"/>
@@ -5723,7 +5892,7 @@
       <c r="AK31" s="53"/>
     </row>
     <row r="32" spans="1:37">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="90" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="15" t="s">
@@ -5750,17 +5919,17 @@
       <c r="I32" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="J32" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="K32" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="L32" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="M32" s="22" t="s">
-        <v>36</v>
+      <c r="J32" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="K32" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="M32" s="56" t="s">
+        <v>35</v>
       </c>
       <c r="N32" s="20" t="s">
         <v>36</v>
@@ -5798,7 +5967,7 @@
       <c r="Y32" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z32" s="58" t="s">
+      <c r="Z32" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA32" s="36"/>
@@ -5814,44 +5983,44 @@
       <c r="AK32" s="36"/>
     </row>
     <row r="33" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A33" s="88"/>
-      <c r="B33" s="89" t="s">
+      <c r="A33" s="91"/>
+      <c r="B33" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="89" t="s">
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G33" s="90"/>
-      <c r="H33" s="90"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="113" t="s">
-        <v>91</v>
-      </c>
-      <c r="K33" s="99"/>
-      <c r="L33" s="99"/>
-      <c r="M33" s="100"/>
-      <c r="N33" s="98" t="s">
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="92" t="s">
+        <v>55</v>
+      </c>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O33" s="99"/>
-      <c r="P33" s="99"/>
-      <c r="Q33" s="100"/>
-      <c r="R33" s="89" t="s">
+      <c r="O33" s="102"/>
+      <c r="P33" s="102"/>
+      <c r="Q33" s="103"/>
+      <c r="R33" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S33" s="90"/>
-      <c r="T33" s="90"/>
-      <c r="U33" s="91"/>
-      <c r="V33" s="89" t="s">
+      <c r="S33" s="93"/>
+      <c r="T33" s="93"/>
+      <c r="U33" s="94"/>
+      <c r="V33" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W33" s="90"/>
-      <c r="X33" s="90"/>
-      <c r="Y33" s="91"/>
-      <c r="Z33" s="61"/>
+      <c r="W33" s="93"/>
+      <c r="X33" s="93"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="64"/>
       <c r="AA33" s="53"/>
       <c r="AB33" s="53"/>
       <c r="AC33" s="53"/>
@@ -5865,7 +6034,7 @@
       <c r="AK33" s="53"/>
     </row>
     <row r="34" spans="1:37">
-      <c r="A34" s="87" t="s">
+      <c r="A34" s="90" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="15" t="s">
@@ -5940,7 +6109,7 @@
       <c r="Y34" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z34" s="58" t="s">
+      <c r="Z34" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA34" s="36"/>
@@ -5956,44 +6125,44 @@
       <c r="AK34" s="36"/>
     </row>
     <row r="35" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A35" s="88"/>
-      <c r="B35" s="89" t="s">
+      <c r="A35" s="91"/>
+      <c r="B35" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="90"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="89" t="s">
+      <c r="C35" s="93"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="90"/>
-      <c r="H35" s="90"/>
-      <c r="I35" s="91"/>
-      <c r="J35" s="89" t="s">
+      <c r="G35" s="93"/>
+      <c r="H35" s="93"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K35" s="90"/>
-      <c r="L35" s="90"/>
-      <c r="M35" s="91"/>
-      <c r="N35" s="98" t="s">
+      <c r="K35" s="93"/>
+      <c r="L35" s="93"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O35" s="99"/>
-      <c r="P35" s="99"/>
-      <c r="Q35" s="100"/>
-      <c r="R35" s="89" t="s">
+      <c r="O35" s="102"/>
+      <c r="P35" s="102"/>
+      <c r="Q35" s="103"/>
+      <c r="R35" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S35" s="90"/>
-      <c r="T35" s="90"/>
-      <c r="U35" s="91"/>
-      <c r="V35" s="89" t="s">
+      <c r="S35" s="93"/>
+      <c r="T35" s="93"/>
+      <c r="U35" s="94"/>
+      <c r="V35" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W35" s="90"/>
-      <c r="X35" s="90"/>
-      <c r="Y35" s="91"/>
-      <c r="Z35" s="61"/>
+      <c r="W35" s="93"/>
+      <c r="X35" s="93"/>
+      <c r="Y35" s="94"/>
+      <c r="Z35" s="64"/>
       <c r="AA35" s="53"/>
       <c r="AB35" s="53"/>
       <c r="AC35" s="53"/>
@@ -6007,7 +6176,7 @@
       <c r="AK35" s="53"/>
     </row>
     <row r="36" spans="1:37">
-      <c r="A36" s="87" t="s">
+      <c r="A36" s="90" t="s">
         <v>13</v>
       </c>
       <c r="B36" s="15" t="s">
@@ -6082,7 +6251,7 @@
       <c r="Y36" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z36" s="58" t="s">
+      <c r="Z36" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA36" s="36"/>
@@ -6098,44 +6267,44 @@
       <c r="AK36" s="36"/>
     </row>
     <row r="37" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A37" s="88"/>
-      <c r="B37" s="89" t="s">
+      <c r="A37" s="91"/>
+      <c r="B37" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="90"/>
-      <c r="D37" s="90"/>
-      <c r="E37" s="91"/>
-      <c r="F37" s="89" t="s">
+      <c r="C37" s="93"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G37" s="90"/>
-      <c r="H37" s="90"/>
-      <c r="I37" s="91"/>
-      <c r="J37" s="89" t="s">
+      <c r="G37" s="93"/>
+      <c r="H37" s="93"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K37" s="90"/>
-      <c r="L37" s="90"/>
-      <c r="M37" s="91"/>
-      <c r="N37" s="98" t="s">
+      <c r="K37" s="93"/>
+      <c r="L37" s="93"/>
+      <c r="M37" s="94"/>
+      <c r="N37" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O37" s="99"/>
-      <c r="P37" s="99"/>
-      <c r="Q37" s="100"/>
-      <c r="R37" s="89" t="s">
+      <c r="O37" s="102"/>
+      <c r="P37" s="102"/>
+      <c r="Q37" s="103"/>
+      <c r="R37" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S37" s="90"/>
-      <c r="T37" s="90"/>
-      <c r="U37" s="91"/>
-      <c r="V37" s="89" t="s">
+      <c r="S37" s="93"/>
+      <c r="T37" s="93"/>
+      <c r="U37" s="94"/>
+      <c r="V37" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W37" s="90"/>
-      <c r="X37" s="90"/>
-      <c r="Y37" s="91"/>
-      <c r="Z37" s="61"/>
+      <c r="W37" s="93"/>
+      <c r="X37" s="93"/>
+      <c r="Y37" s="94"/>
+      <c r="Z37" s="64"/>
       <c r="AA37" s="53"/>
       <c r="AB37" s="53"/>
       <c r="AC37" s="53"/>
@@ -6149,7 +6318,7 @@
       <c r="AK37" s="53"/>
     </row>
     <row r="38" spans="1:37">
-      <c r="A38" s="87" t="s">
+      <c r="A38" s="90" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="15" t="s">
@@ -6224,7 +6393,7 @@
       <c r="Y38" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z38" s="58" t="s">
+      <c r="Z38" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA38" s="36"/>
@@ -6240,44 +6409,44 @@
       <c r="AK38" s="36"/>
     </row>
     <row r="39" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A39" s="88"/>
-      <c r="B39" s="89" t="s">
+      <c r="A39" s="91"/>
+      <c r="B39" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="91"/>
-      <c r="F39" s="89" t="s">
+      <c r="C39" s="93"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="94"/>
+      <c r="F39" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G39" s="90"/>
-      <c r="H39" s="90"/>
-      <c r="I39" s="91"/>
-      <c r="J39" s="89" t="s">
+      <c r="G39" s="93"/>
+      <c r="H39" s="93"/>
+      <c r="I39" s="94"/>
+      <c r="J39" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K39" s="90"/>
-      <c r="L39" s="90"/>
-      <c r="M39" s="91"/>
-      <c r="N39" s="98" t="s">
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="94"/>
+      <c r="N39" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O39" s="99"/>
-      <c r="P39" s="99"/>
-      <c r="Q39" s="100"/>
-      <c r="R39" s="89" t="s">
+      <c r="O39" s="102"/>
+      <c r="P39" s="102"/>
+      <c r="Q39" s="103"/>
+      <c r="R39" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S39" s="90"/>
-      <c r="T39" s="90"/>
-      <c r="U39" s="91"/>
-      <c r="V39" s="89" t="s">
+      <c r="S39" s="93"/>
+      <c r="T39" s="93"/>
+      <c r="U39" s="94"/>
+      <c r="V39" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W39" s="90"/>
-      <c r="X39" s="90"/>
-      <c r="Y39" s="91"/>
-      <c r="Z39" s="61"/>
+      <c r="W39" s="93"/>
+      <c r="X39" s="93"/>
+      <c r="Y39" s="94"/>
+      <c r="Z39" s="64"/>
       <c r="AA39" s="53"/>
       <c r="AB39" s="53"/>
       <c r="AC39" s="53"/>
@@ -6291,7 +6460,7 @@
       <c r="AK39" s="53"/>
     </row>
     <row r="40" spans="1:37">
-      <c r="A40" s="87" t="s">
+      <c r="A40" s="90" t="s">
         <v>15</v>
       </c>
       <c r="B40" s="15" t="s">
@@ -6366,7 +6535,7 @@
       <c r="Y40" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z40" s="58" t="s">
+      <c r="Z40" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA40" s="36"/>
@@ -6382,44 +6551,44 @@
       <c r="AK40" s="36"/>
     </row>
     <row r="41" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A41" s="88"/>
-      <c r="B41" s="89" t="s">
+      <c r="A41" s="91"/>
+      <c r="B41" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-      <c r="E41" s="91"/>
-      <c r="F41" s="89" t="s">
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="91"/>
-      <c r="J41" s="89" t="s">
+      <c r="G41" s="93"/>
+      <c r="H41" s="93"/>
+      <c r="I41" s="94"/>
+      <c r="J41" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K41" s="90"/>
-      <c r="L41" s="90"/>
-      <c r="M41" s="91"/>
-      <c r="N41" s="98" t="s">
+      <c r="K41" s="93"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="94"/>
+      <c r="N41" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O41" s="99"/>
-      <c r="P41" s="99"/>
-      <c r="Q41" s="100"/>
-      <c r="R41" s="89" t="s">
+      <c r="O41" s="102"/>
+      <c r="P41" s="102"/>
+      <c r="Q41" s="103"/>
+      <c r="R41" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S41" s="90"/>
-      <c r="T41" s="90"/>
-      <c r="U41" s="91"/>
-      <c r="V41" s="89" t="s">
+      <c r="S41" s="93"/>
+      <c r="T41" s="93"/>
+      <c r="U41" s="94"/>
+      <c r="V41" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W41" s="90"/>
-      <c r="X41" s="90"/>
-      <c r="Y41" s="91"/>
-      <c r="Z41" s="61"/>
+      <c r="W41" s="93"/>
+      <c r="X41" s="93"/>
+      <c r="Y41" s="94"/>
+      <c r="Z41" s="64"/>
       <c r="AA41" s="53"/>
       <c r="AB41" s="53"/>
       <c r="AC41" s="53"/>
@@ -6433,7 +6602,7 @@
       <c r="AK41" s="53"/>
     </row>
     <row r="42" spans="1:37">
-      <c r="A42" s="87" t="s">
+      <c r="A42" s="90" t="s">
         <v>16</v>
       </c>
       <c r="B42" s="15" t="s">
@@ -6508,7 +6677,7 @@
       <c r="Y42" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z42" s="58" t="s">
+      <c r="Z42" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA42" s="36"/>
@@ -6524,44 +6693,44 @@
       <c r="AK42" s="36"/>
     </row>
     <row r="43" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A43" s="88"/>
-      <c r="B43" s="89" t="s">
+      <c r="A43" s="91"/>
+      <c r="B43" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="90"/>
-      <c r="D43" s="90"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="89" t="s">
+      <c r="C43" s="93"/>
+      <c r="D43" s="93"/>
+      <c r="E43" s="94"/>
+      <c r="F43" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G43" s="90"/>
-      <c r="H43" s="90"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="89" t="s">
+      <c r="G43" s="93"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="94"/>
+      <c r="J43" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K43" s="90"/>
-      <c r="L43" s="90"/>
-      <c r="M43" s="91"/>
-      <c r="N43" s="98" t="s">
+      <c r="K43" s="93"/>
+      <c r="L43" s="93"/>
+      <c r="M43" s="94"/>
+      <c r="N43" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O43" s="99"/>
-      <c r="P43" s="99"/>
-      <c r="Q43" s="100"/>
-      <c r="R43" s="89" t="s">
+      <c r="O43" s="102"/>
+      <c r="P43" s="102"/>
+      <c r="Q43" s="103"/>
+      <c r="R43" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S43" s="90"/>
-      <c r="T43" s="90"/>
-      <c r="U43" s="91"/>
-      <c r="V43" s="89" t="s">
+      <c r="S43" s="93"/>
+      <c r="T43" s="93"/>
+      <c r="U43" s="94"/>
+      <c r="V43" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W43" s="90"/>
-      <c r="X43" s="90"/>
-      <c r="Y43" s="91"/>
-      <c r="Z43" s="61"/>
+      <c r="W43" s="93"/>
+      <c r="X43" s="93"/>
+      <c r="Y43" s="94"/>
+      <c r="Z43" s="64"/>
       <c r="AA43" s="53"/>
       <c r="AB43" s="53"/>
       <c r="AC43" s="53"/>
@@ -6575,7 +6744,7 @@
       <c r="AK43" s="53"/>
     </row>
     <row r="44" spans="1:37">
-      <c r="A44" s="87" t="s">
+      <c r="A44" s="90" t="s">
         <v>17</v>
       </c>
       <c r="B44" s="20" t="s">
@@ -6650,7 +6819,7 @@
       <c r="Y44" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z44" s="58" t="s">
+      <c r="Z44" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA44" s="36"/>
@@ -6666,44 +6835,44 @@
       <c r="AK44" s="36"/>
     </row>
     <row r="45" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A45" s="88"/>
-      <c r="B45" s="89" t="s">
+      <c r="A45" s="91"/>
+      <c r="B45" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="90"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="89" t="s">
+      <c r="C45" s="93"/>
+      <c r="D45" s="93"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G45" s="90"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="91"/>
-      <c r="J45" s="89" t="s">
+      <c r="G45" s="93"/>
+      <c r="H45" s="93"/>
+      <c r="I45" s="94"/>
+      <c r="J45" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K45" s="90"/>
-      <c r="L45" s="90"/>
-      <c r="M45" s="91"/>
-      <c r="N45" s="98" t="s">
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
+      <c r="M45" s="94"/>
+      <c r="N45" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O45" s="99"/>
-      <c r="P45" s="99"/>
-      <c r="Q45" s="100"/>
-      <c r="R45" s="89" t="s">
+      <c r="O45" s="102"/>
+      <c r="P45" s="102"/>
+      <c r="Q45" s="103"/>
+      <c r="R45" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S45" s="90"/>
-      <c r="T45" s="90"/>
-      <c r="U45" s="91"/>
-      <c r="V45" s="89" t="s">
+      <c r="S45" s="93"/>
+      <c r="T45" s="93"/>
+      <c r="U45" s="94"/>
+      <c r="V45" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W45" s="90"/>
-      <c r="X45" s="90"/>
-      <c r="Y45" s="91"/>
-      <c r="Z45" s="61"/>
+      <c r="W45" s="93"/>
+      <c r="X45" s="93"/>
+      <c r="Y45" s="94"/>
+      <c r="Z45" s="64"/>
       <c r="AA45" s="53"/>
       <c r="AB45" s="53"/>
       <c r="AC45" s="53"/>
@@ -6717,7 +6886,7 @@
       <c r="AK45" s="53"/>
     </row>
     <row r="46" spans="1:37">
-      <c r="A46" s="87" t="s">
+      <c r="A46" s="90" t="s">
         <v>18</v>
       </c>
       <c r="B46" s="20" t="s">
@@ -6792,7 +6961,7 @@
       <c r="Y46" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z46" s="58" t="s">
+      <c r="Z46" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA46" s="36"/>
@@ -6808,44 +6977,44 @@
       <c r="AK46" s="36"/>
     </row>
     <row r="47" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A47" s="88"/>
-      <c r="B47" s="89" t="s">
+      <c r="A47" s="91"/>
+      <c r="B47" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="89" t="s">
+      <c r="C47" s="93"/>
+      <c r="D47" s="93"/>
+      <c r="E47" s="94"/>
+      <c r="F47" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G47" s="90"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="91"/>
-      <c r="J47" s="89" t="s">
+      <c r="G47" s="93"/>
+      <c r="H47" s="93"/>
+      <c r="I47" s="94"/>
+      <c r="J47" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K47" s="90"/>
-      <c r="L47" s="90"/>
-      <c r="M47" s="91"/>
-      <c r="N47" s="98" t="s">
+      <c r="K47" s="93"/>
+      <c r="L47" s="93"/>
+      <c r="M47" s="94"/>
+      <c r="N47" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O47" s="99"/>
-      <c r="P47" s="99"/>
-      <c r="Q47" s="100"/>
-      <c r="R47" s="89" t="s">
+      <c r="O47" s="102"/>
+      <c r="P47" s="102"/>
+      <c r="Q47" s="103"/>
+      <c r="R47" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S47" s="90"/>
-      <c r="T47" s="90"/>
-      <c r="U47" s="91"/>
-      <c r="V47" s="89" t="s">
+      <c r="S47" s="93"/>
+      <c r="T47" s="93"/>
+      <c r="U47" s="94"/>
+      <c r="V47" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W47" s="90"/>
-      <c r="X47" s="90"/>
-      <c r="Y47" s="91"/>
-      <c r="Z47" s="61"/>
+      <c r="W47" s="93"/>
+      <c r="X47" s="93"/>
+      <c r="Y47" s="94"/>
+      <c r="Z47" s="64"/>
       <c r="AA47" s="53"/>
       <c r="AB47" s="53"/>
       <c r="AC47" s="53"/>
@@ -6859,7 +7028,7 @@
       <c r="AK47" s="53"/>
     </row>
     <row r="48" spans="1:37">
-      <c r="A48" s="87" t="s">
+      <c r="A48" s="90" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="15" t="s">
@@ -6934,7 +7103,7 @@
       <c r="Y48" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z48" s="58" t="s">
+      <c r="Z48" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA48" s="36"/>
@@ -6950,44 +7119,44 @@
       <c r="AK48" s="36"/>
     </row>
     <row r="49" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A49" s="88"/>
-      <c r="B49" s="89" t="s">
+      <c r="A49" s="91"/>
+      <c r="B49" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="89" t="s">
+      <c r="C49" s="93"/>
+      <c r="D49" s="93"/>
+      <c r="E49" s="94"/>
+      <c r="F49" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
-      <c r="I49" s="91"/>
-      <c r="J49" s="89" t="s">
+      <c r="G49" s="93"/>
+      <c r="H49" s="93"/>
+      <c r="I49" s="94"/>
+      <c r="J49" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K49" s="90"/>
-      <c r="L49" s="90"/>
-      <c r="M49" s="91"/>
-      <c r="N49" s="98" t="s">
+      <c r="K49" s="93"/>
+      <c r="L49" s="93"/>
+      <c r="M49" s="94"/>
+      <c r="N49" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O49" s="99"/>
-      <c r="P49" s="99"/>
-      <c r="Q49" s="100"/>
-      <c r="R49" s="89" t="s">
+      <c r="O49" s="102"/>
+      <c r="P49" s="102"/>
+      <c r="Q49" s="103"/>
+      <c r="R49" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S49" s="90"/>
-      <c r="T49" s="90"/>
-      <c r="U49" s="91"/>
-      <c r="V49" s="89" t="s">
+      <c r="S49" s="93"/>
+      <c r="T49" s="93"/>
+      <c r="U49" s="94"/>
+      <c r="V49" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W49" s="90"/>
-      <c r="X49" s="90"/>
-      <c r="Y49" s="91"/>
-      <c r="Z49" s="61"/>
+      <c r="W49" s="93"/>
+      <c r="X49" s="93"/>
+      <c r="Y49" s="94"/>
+      <c r="Z49" s="64"/>
       <c r="AA49" s="53"/>
       <c r="AB49" s="53"/>
       <c r="AC49" s="53"/>
@@ -7001,7 +7170,7 @@
       <c r="AK49" s="53"/>
     </row>
     <row r="50" spans="1:37">
-      <c r="A50" s="87" t="s">
+      <c r="A50" s="90" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="15" t="s">
@@ -7076,7 +7245,7 @@
       <c r="Y50" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z50" s="58" t="s">
+      <c r="Z50" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA50" s="36"/>
@@ -7092,44 +7261,44 @@
       <c r="AK50" s="36"/>
     </row>
     <row r="51" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A51" s="88"/>
-      <c r="B51" s="89" t="s">
+      <c r="A51" s="91"/>
+      <c r="B51" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="91"/>
-      <c r="F51" s="89" t="s">
+      <c r="C51" s="93"/>
+      <c r="D51" s="93"/>
+      <c r="E51" s="94"/>
+      <c r="F51" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G51" s="90"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="91"/>
-      <c r="J51" s="89" t="s">
+      <c r="G51" s="93"/>
+      <c r="H51" s="93"/>
+      <c r="I51" s="94"/>
+      <c r="J51" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K51" s="90"/>
-      <c r="L51" s="90"/>
-      <c r="M51" s="91"/>
-      <c r="N51" s="98" t="s">
+      <c r="K51" s="93"/>
+      <c r="L51" s="93"/>
+      <c r="M51" s="94"/>
+      <c r="N51" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O51" s="99"/>
-      <c r="P51" s="99"/>
-      <c r="Q51" s="100"/>
-      <c r="R51" s="89" t="s">
+      <c r="O51" s="102"/>
+      <c r="P51" s="102"/>
+      <c r="Q51" s="103"/>
+      <c r="R51" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S51" s="90"/>
-      <c r="T51" s="90"/>
-      <c r="U51" s="91"/>
-      <c r="V51" s="89" t="s">
+      <c r="S51" s="93"/>
+      <c r="T51" s="93"/>
+      <c r="U51" s="94"/>
+      <c r="V51" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W51" s="90"/>
-      <c r="X51" s="90"/>
-      <c r="Y51" s="91"/>
-      <c r="Z51" s="61"/>
+      <c r="W51" s="93"/>
+      <c r="X51" s="93"/>
+      <c r="Y51" s="94"/>
+      <c r="Z51" s="64"/>
       <c r="AA51" s="53"/>
       <c r="AB51" s="53"/>
       <c r="AC51" s="53"/>
@@ -7143,7 +7312,7 @@
       <c r="AK51" s="53"/>
     </row>
     <row r="52" spans="1:37">
-      <c r="A52" s="87" t="s">
+      <c r="A52" s="90" t="s">
         <v>21</v>
       </c>
       <c r="B52" s="20" t="s">
@@ -7218,7 +7387,7 @@
       <c r="Y52" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z52" s="58" t="s">
+      <c r="Z52" s="61" t="s">
         <v>50</v>
       </c>
       <c r="AA52" s="36"/>
@@ -7234,44 +7403,44 @@
       <c r="AK52" s="36"/>
     </row>
     <row r="53" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A53" s="88"/>
-      <c r="B53" s="89" t="s">
+      <c r="A53" s="91"/>
+      <c r="B53" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C53" s="90"/>
-      <c r="D53" s="90"/>
-      <c r="E53" s="91"/>
-      <c r="F53" s="89" t="s">
+      <c r="C53" s="93"/>
+      <c r="D53" s="93"/>
+      <c r="E53" s="94"/>
+      <c r="F53" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G53" s="90"/>
-      <c r="H53" s="90"/>
-      <c r="I53" s="91"/>
-      <c r="J53" s="89" t="s">
+      <c r="G53" s="93"/>
+      <c r="H53" s="93"/>
+      <c r="I53" s="94"/>
+      <c r="J53" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="K53" s="90"/>
-      <c r="L53" s="90"/>
-      <c r="M53" s="91"/>
-      <c r="N53" s="98" t="s">
+      <c r="K53" s="93"/>
+      <c r="L53" s="93"/>
+      <c r="M53" s="94"/>
+      <c r="N53" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O53" s="99"/>
-      <c r="P53" s="99"/>
-      <c r="Q53" s="100"/>
-      <c r="R53" s="89" t="s">
+      <c r="O53" s="102"/>
+      <c r="P53" s="102"/>
+      <c r="Q53" s="103"/>
+      <c r="R53" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S53" s="90"/>
-      <c r="T53" s="90"/>
-      <c r="U53" s="91"/>
-      <c r="V53" s="89" t="s">
+      <c r="S53" s="93"/>
+      <c r="T53" s="93"/>
+      <c r="U53" s="94"/>
+      <c r="V53" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W53" s="90"/>
-      <c r="X53" s="90"/>
-      <c r="Y53" s="91"/>
-      <c r="Z53" s="61"/>
+      <c r="W53" s="93"/>
+      <c r="X53" s="93"/>
+      <c r="Y53" s="94"/>
+      <c r="Z53" s="64"/>
       <c r="AA53" s="53"/>
       <c r="AB53" s="53"/>
       <c r="AC53" s="53"/>
@@ -7285,7 +7454,7 @@
       <c r="AK53" s="53"/>
     </row>
     <row r="54" spans="1:37">
-      <c r="A54" s="87" t="s">
+      <c r="A54" s="90" t="s">
         <v>22</v>
       </c>
       <c r="B54" s="20" t="s">
@@ -7360,7 +7529,7 @@
       <c r="Y54" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z54" s="58" t="s">
+      <c r="Z54" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA54" s="36"/>
@@ -7376,44 +7545,44 @@
       <c r="AK54" s="36"/>
     </row>
     <row r="55" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1">
-      <c r="A55" s="88"/>
-      <c r="B55" s="89" t="s">
+      <c r="A55" s="91"/>
+      <c r="B55" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="90"/>
-      <c r="D55" s="90"/>
-      <c r="E55" s="91"/>
-      <c r="F55" s="89" t="s">
+      <c r="C55" s="93"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="94"/>
+      <c r="F55" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="G55" s="90"/>
-      <c r="H55" s="90"/>
-      <c r="I55" s="91"/>
-      <c r="J55" s="104" t="s">
+      <c r="G55" s="93"/>
+      <c r="H55" s="93"/>
+      <c r="I55" s="94"/>
+      <c r="J55" s="107" t="s">
         <v>55</v>
       </c>
-      <c r="K55" s="105"/>
-      <c r="L55" s="105"/>
-      <c r="M55" s="106"/>
-      <c r="N55" s="98" t="s">
+      <c r="K55" s="108"/>
+      <c r="L55" s="108"/>
+      <c r="M55" s="109"/>
+      <c r="N55" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O55" s="99"/>
-      <c r="P55" s="99"/>
-      <c r="Q55" s="100"/>
-      <c r="R55" s="89" t="s">
+      <c r="O55" s="102"/>
+      <c r="P55" s="102"/>
+      <c r="Q55" s="103"/>
+      <c r="R55" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="S55" s="90"/>
-      <c r="T55" s="90"/>
-      <c r="U55" s="91"/>
-      <c r="V55" s="89" t="s">
+      <c r="S55" s="93"/>
+      <c r="T55" s="93"/>
+      <c r="U55" s="94"/>
+      <c r="V55" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="W55" s="90"/>
-      <c r="X55" s="90"/>
-      <c r="Y55" s="91"/>
-      <c r="Z55" s="61"/>
+      <c r="W55" s="93"/>
+      <c r="X55" s="93"/>
+      <c r="Y55" s="94"/>
+      <c r="Z55" s="64"/>
       <c r="AA55" s="53"/>
       <c r="AB55" s="53"/>
       <c r="AC55" s="53"/>
@@ -7427,7 +7596,7 @@
       <c r="AK55" s="53"/>
     </row>
     <row r="56" spans="1:37">
-      <c r="A56" s="87" t="s">
+      <c r="A56" s="90" t="s">
         <v>23</v>
       </c>
       <c r="B56" s="20" t="s">
@@ -7502,7 +7671,7 @@
       <c r="Y56" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Z56" s="58" t="s">
+      <c r="Z56" s="61" t="s">
         <v>45</v>
       </c>
       <c r="AA56" s="36"/>
@@ -7518,44 +7687,44 @@
       <c r="AK56" s="36"/>
     </row>
     <row r="57" spans="1:37" s="19" customFormat="1" ht="23" customHeight="1" thickBot="1">
-      <c r="A57" s="87"/>
-      <c r="B57" s="101" t="s">
+      <c r="A57" s="90"/>
+      <c r="B57" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="102"/>
-      <c r="D57" s="102"/>
-      <c r="E57" s="103"/>
-      <c r="F57" s="101" t="s">
+      <c r="C57" s="105"/>
+      <c r="D57" s="105"/>
+      <c r="E57" s="106"/>
+      <c r="F57" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="G57" s="102"/>
-      <c r="H57" s="102"/>
-      <c r="I57" s="103"/>
-      <c r="J57" s="110" t="s">
+      <c r="G57" s="105"/>
+      <c r="H57" s="105"/>
+      <c r="I57" s="106"/>
+      <c r="J57" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="K57" s="111"/>
-      <c r="L57" s="111"/>
-      <c r="M57" s="112"/>
-      <c r="N57" s="107" t="s">
+      <c r="K57" s="114"/>
+      <c r="L57" s="114"/>
+      <c r="M57" s="115"/>
+      <c r="N57" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="O57" s="108"/>
-      <c r="P57" s="108"/>
-      <c r="Q57" s="109"/>
-      <c r="R57" s="101" t="s">
+      <c r="O57" s="111"/>
+      <c r="P57" s="111"/>
+      <c r="Q57" s="112"/>
+      <c r="R57" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="S57" s="102"/>
-      <c r="T57" s="102"/>
-      <c r="U57" s="103"/>
-      <c r="V57" s="101" t="s">
+      <c r="S57" s="105"/>
+      <c r="T57" s="105"/>
+      <c r="U57" s="106"/>
+      <c r="V57" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="W57" s="102"/>
-      <c r="X57" s="102"/>
-      <c r="Y57" s="103"/>
-      <c r="Z57" s="58"/>
+      <c r="W57" s="105"/>
+      <c r="X57" s="105"/>
+      <c r="Y57" s="106"/>
+      <c r="Z57" s="61"/>
       <c r="AA57" s="53"/>
       <c r="AB57" s="53"/>
       <c r="AC57" s="53"/>
@@ -7569,46 +7738,46 @@
       <c r="AK57" s="53"/>
     </row>
     <row r="58" spans="1:37">
-      <c r="A58" s="79" t="s">
+      <c r="A58" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="81" t="s">
+      <c r="B58" s="84" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" s="85"/>
+      <c r="D58" s="85"/>
+      <c r="E58" s="86"/>
+      <c r="F58" s="84" t="s">
+        <v>44</v>
+      </c>
+      <c r="G58" s="85"/>
+      <c r="H58" s="85"/>
+      <c r="I58" s="86"/>
+      <c r="J58" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="C58" s="82"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="83"/>
-      <c r="F58" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="G58" s="82"/>
-      <c r="H58" s="82"/>
-      <c r="I58" s="83"/>
-      <c r="J58" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="K58" s="82"/>
-      <c r="L58" s="82"/>
-      <c r="M58" s="83"/>
-      <c r="N58" s="81" t="s">
+      <c r="K58" s="85"/>
+      <c r="L58" s="85"/>
+      <c r="M58" s="86"/>
+      <c r="N58" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="O58" s="82"/>
-      <c r="P58" s="82"/>
-      <c r="Q58" s="83"/>
-      <c r="R58" s="81" t="s">
+      <c r="O58" s="85"/>
+      <c r="P58" s="85"/>
+      <c r="Q58" s="86"/>
+      <c r="R58" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="S58" s="82"/>
-      <c r="T58" s="82"/>
-      <c r="U58" s="83"/>
-      <c r="V58" s="81" t="s">
+      <c r="S58" s="85"/>
+      <c r="T58" s="85"/>
+      <c r="U58" s="86"/>
+      <c r="V58" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="W58" s="82"/>
-      <c r="X58" s="82"/>
-      <c r="Y58" s="83"/>
-      <c r="Z58" s="95" t="s">
+      <c r="W58" s="85"/>
+      <c r="X58" s="85"/>
+      <c r="Y58" s="86"/>
+      <c r="Z58" s="98" t="s">
         <v>50</v>
       </c>
       <c r="AA58" s="36"/>
@@ -7624,32 +7793,32 @@
       <c r="AK58" s="36"/>
     </row>
     <row r="59" spans="1:37" ht="16" thickBot="1">
-      <c r="A59" s="80"/>
-      <c r="B59" s="59"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="59"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="60"/>
-      <c r="I59" s="61"/>
-      <c r="J59" s="59"/>
-      <c r="K59" s="60"/>
-      <c r="L59" s="60"/>
-      <c r="M59" s="61"/>
-      <c r="N59" s="59"/>
-      <c r="O59" s="60"/>
-      <c r="P59" s="60"/>
-      <c r="Q59" s="61"/>
-      <c r="R59" s="59"/>
-      <c r="S59" s="60"/>
-      <c r="T59" s="60"/>
-      <c r="U59" s="61"/>
-      <c r="V59" s="59"/>
-      <c r="W59" s="60"/>
-      <c r="X59" s="60"/>
-      <c r="Y59" s="61"/>
-      <c r="Z59" s="96"/>
+      <c r="A59" s="70"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="64"/>
+      <c r="J59" s="62"/>
+      <c r="K59" s="63"/>
+      <c r="L59" s="63"/>
+      <c r="M59" s="64"/>
+      <c r="N59" s="62"/>
+      <c r="O59" s="63"/>
+      <c r="P59" s="63"/>
+      <c r="Q59" s="64"/>
+      <c r="R59" s="62"/>
+      <c r="S59" s="63"/>
+      <c r="T59" s="63"/>
+      <c r="U59" s="64"/>
+      <c r="V59" s="62"/>
+      <c r="W59" s="63"/>
+      <c r="X59" s="63"/>
+      <c r="Y59" s="64"/>
+      <c r="Z59" s="99"/>
       <c r="AA59" s="36"/>
       <c r="AB59" s="36"/>
       <c r="AC59" s="36"/>
@@ -7663,46 +7832,46 @@
       <c r="AK59" s="36"/>
     </row>
     <row r="60" spans="1:37">
-      <c r="A60" s="65" t="s">
+      <c r="A60" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" s="60"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="G60" s="60"/>
+      <c r="H60" s="60"/>
+      <c r="I60" s="61"/>
+      <c r="J60" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="56" t="s">
+      <c r="K60" s="60"/>
+      <c r="L60" s="60"/>
+      <c r="M60" s="61"/>
+      <c r="N60" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="G60" s="57"/>
-      <c r="H60" s="57"/>
-      <c r="I60" s="58"/>
-      <c r="J60" s="56" t="s">
+      <c r="O60" s="60"/>
+      <c r="P60" s="60"/>
+      <c r="Q60" s="61"/>
+      <c r="R60" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="K60" s="57"/>
-      <c r="L60" s="57"/>
-      <c r="M60" s="58"/>
-      <c r="N60" s="56" t="s">
+      <c r="S60" s="60"/>
+      <c r="T60" s="60"/>
+      <c r="U60" s="61"/>
+      <c r="V60" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="O60" s="57"/>
-      <c r="P60" s="57"/>
-      <c r="Q60" s="58"/>
-      <c r="R60" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="S60" s="57"/>
-      <c r="T60" s="57"/>
-      <c r="U60" s="58"/>
-      <c r="V60" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="W60" s="57"/>
-      <c r="X60" s="57"/>
-      <c r="Y60" s="58"/>
-      <c r="Z60" s="95" t="s">
+      <c r="W60" s="60"/>
+      <c r="X60" s="60"/>
+      <c r="Y60" s="61"/>
+      <c r="Z60" s="98" t="s">
         <v>51</v>
       </c>
       <c r="AA60" s="36"/>
@@ -7718,32 +7887,32 @@
       <c r="AK60" s="36"/>
     </row>
     <row r="61" spans="1:37" ht="16" thickBot="1">
-      <c r="A61" s="80"/>
-      <c r="B61" s="59"/>
-      <c r="C61" s="60"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="59"/>
-      <c r="G61" s="60"/>
-      <c r="H61" s="60"/>
-      <c r="I61" s="61"/>
-      <c r="J61" s="59"/>
-      <c r="K61" s="60"/>
-      <c r="L61" s="60"/>
-      <c r="M61" s="61"/>
-      <c r="N61" s="59"/>
-      <c r="O61" s="60"/>
-      <c r="P61" s="60"/>
-      <c r="Q61" s="61"/>
-      <c r="R61" s="59"/>
-      <c r="S61" s="60"/>
-      <c r="T61" s="60"/>
-      <c r="U61" s="61"/>
-      <c r="V61" s="59"/>
-      <c r="W61" s="60"/>
-      <c r="X61" s="60"/>
-      <c r="Y61" s="61"/>
-      <c r="Z61" s="96"/>
+      <c r="A61" s="70"/>
+      <c r="B61" s="62"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="62"/>
+      <c r="G61" s="63"/>
+      <c r="H61" s="63"/>
+      <c r="I61" s="64"/>
+      <c r="J61" s="62"/>
+      <c r="K61" s="63"/>
+      <c r="L61" s="63"/>
+      <c r="M61" s="64"/>
+      <c r="N61" s="62"/>
+      <c r="O61" s="63"/>
+      <c r="P61" s="63"/>
+      <c r="Q61" s="64"/>
+      <c r="R61" s="62"/>
+      <c r="S61" s="63"/>
+      <c r="T61" s="63"/>
+      <c r="U61" s="64"/>
+      <c r="V61" s="62"/>
+      <c r="W61" s="63"/>
+      <c r="X61" s="63"/>
+      <c r="Y61" s="64"/>
+      <c r="Z61" s="99"/>
       <c r="AA61" s="36"/>
       <c r="AB61" s="36"/>
       <c r="AC61" s="36"/>
@@ -7848,46 +8017,46 @@
       <c r="AK62" s="36"/>
     </row>
     <row r="63" spans="1:37">
-      <c r="A63" s="65" t="s">
+      <c r="A63" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C63" s="57"/>
-      <c r="D63" s="57"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="56" t="s">
+      <c r="C63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="61"/>
+      <c r="F63" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="G63" s="57"/>
-      <c r="H63" s="57"/>
-      <c r="I63" s="58"/>
-      <c r="J63" s="56" t="s">
+      <c r="G63" s="60"/>
+      <c r="H63" s="60"/>
+      <c r="I63" s="61"/>
+      <c r="J63" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="K63" s="57"/>
-      <c r="L63" s="57"/>
-      <c r="M63" s="58"/>
-      <c r="N63" s="56" t="s">
+      <c r="K63" s="60"/>
+      <c r="L63" s="60"/>
+      <c r="M63" s="61"/>
+      <c r="N63" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="O63" s="57"/>
-      <c r="P63" s="57"/>
-      <c r="Q63" s="58"/>
-      <c r="R63" s="56" t="s">
+      <c r="O63" s="60"/>
+      <c r="P63" s="60"/>
+      <c r="Q63" s="61"/>
+      <c r="R63" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="S63" s="57"/>
-      <c r="T63" s="57"/>
-      <c r="U63" s="58"/>
-      <c r="V63" s="56" t="s">
+      <c r="S63" s="60"/>
+      <c r="T63" s="60"/>
+      <c r="U63" s="61"/>
+      <c r="V63" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="W63" s="57"/>
-      <c r="X63" s="57"/>
-      <c r="Y63" s="58"/>
-      <c r="Z63" s="58" t="s">
+      <c r="W63" s="60"/>
+      <c r="X63" s="60"/>
+      <c r="Y63" s="61"/>
+      <c r="Z63" s="61" t="s">
         <v>47</v>
       </c>
       <c r="AA63" s="36"/>
@@ -7903,32 +8072,32 @@
       <c r="AK63" s="36"/>
     </row>
     <row r="64" spans="1:37" ht="16" thickBot="1">
-      <c r="A64" s="66"/>
-      <c r="B64" s="62"/>
-      <c r="C64" s="63"/>
-      <c r="D64" s="63"/>
-      <c r="E64" s="64"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="63"/>
-      <c r="H64" s="63"/>
-      <c r="I64" s="64"/>
-      <c r="J64" s="62"/>
-      <c r="K64" s="63"/>
-      <c r="L64" s="63"/>
-      <c r="M64" s="64"/>
-      <c r="N64" s="62"/>
-      <c r="O64" s="63"/>
-      <c r="P64" s="63"/>
-      <c r="Q64" s="64"/>
-      <c r="R64" s="62"/>
-      <c r="S64" s="63"/>
-      <c r="T64" s="63"/>
-      <c r="U64" s="64"/>
-      <c r="V64" s="62"/>
-      <c r="W64" s="63"/>
-      <c r="X64" s="63"/>
-      <c r="Y64" s="64"/>
-      <c r="Z64" s="64"/>
+      <c r="A64" s="69"/>
+      <c r="B64" s="65"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="65"/>
+      <c r="G64" s="66"/>
+      <c r="H64" s="66"/>
+      <c r="I64" s="67"/>
+      <c r="J64" s="65"/>
+      <c r="K64" s="66"/>
+      <c r="L64" s="66"/>
+      <c r="M64" s="67"/>
+      <c r="N64" s="65"/>
+      <c r="O64" s="66"/>
+      <c r="P64" s="66"/>
+      <c r="Q64" s="67"/>
+      <c r="R64" s="65"/>
+      <c r="S64" s="66"/>
+      <c r="T64" s="66"/>
+      <c r="U64" s="67"/>
+      <c r="V64" s="65"/>
+      <c r="W64" s="66"/>
+      <c r="X64" s="66"/>
+      <c r="Y64" s="67"/>
+      <c r="Z64" s="67"/>
       <c r="AA64" s="36"/>
       <c r="AB64" s="36"/>
       <c r="AC64" s="36"/>
@@ -10335,770 +10504,781 @@
     <mergeCell ref="R63:U64"/>
     <mergeCell ref="V63:Y64"/>
   </mergeCells>
-  <conditionalFormatting sqref="B10:M10 B11 F11 R11 V11 B12:M12 B20:M20 B24:M24 B26:M26 B32:M32 B14:M14 B16:M16 B18:M18 B22:M22 B28:M28 B30:M30 B34:M34 B38:M38 B40:M40 B42:M42 B44:M44 B46:M46 B48:M48 B50:M50 B54:M54 B56:M56 B36:M36 B52:M52">
-    <cfRule type="containsText" dxfId="208" priority="314" operator="containsText" text="┄">
+  <conditionalFormatting sqref="B10:M10 B11 F11 R11 V11 B12:M12 B20:M20 B24:M24 B26:M26 B14:M14 B16:M16 B18:M18 B22:M22 B28:M28 B30:M30 B34:M34 B38:M38 B40:M40 B42:M42 B44:M44 B46:M46 B48:M48 B50:M50 B54:M54 B56:M56 B36:M36 B52:M52 B32:M32">
+    <cfRule type="containsText" dxfId="223" priority="320" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="315" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="222" priority="321" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="316" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="221" priority="322" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60:Y62">
-    <cfRule type="containsText" dxfId="205" priority="310" operator="containsText" text="IN-PROGRESS">
+    <cfRule type="containsText" dxfId="220" priority="316" operator="containsText" text="IN-PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN-PROGRESS",B60)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="311" operator="containsText" text="COMPLETED">
+    <cfRule type="containsText" dxfId="219" priority="317" operator="containsText" text="COMPLETED">
       <formula>NOT(ISERROR(SEARCH("COMPLETED",B60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:Y64 Z62">
-    <cfRule type="containsText" dxfId="203" priority="304" operator="containsText" text="INCOMPLETE">
+    <cfRule type="containsText" dxfId="218" priority="310" operator="containsText" text="INCOMPLETE">
       <formula>NOT(ISERROR(SEARCH("INCOMPLETE",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="305" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="217" priority="311" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z60:Z61">
-    <cfRule type="containsText" dxfId="201" priority="303" operator="containsText" text="IN-PROGRESS">
+    <cfRule type="containsText" dxfId="216" priority="309" operator="containsText" text="IN-PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN-PROGRESS",Z60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z10:Z57 B58:Z59">
-    <cfRule type="containsText" dxfId="200" priority="300" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="215" priority="306" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="301" operator="containsText" text="PARTIALLY">
+    <cfRule type="containsText" dxfId="214" priority="307" operator="containsText" text="PARTIALLY">
       <formula>NOT(ISERROR(SEARCH("PARTIALLY",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="302" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="213" priority="308" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21 F21 R21 V21">
-    <cfRule type="containsText" dxfId="197" priority="285" operator="containsText" text="┄">
+  <conditionalFormatting sqref="B21 R21 V21">
+    <cfRule type="containsText" dxfId="212" priority="291" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="286" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="211" priority="292" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="287" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="210" priority="293" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13 R13 V13">
-    <cfRule type="containsText" dxfId="194" priority="294" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="209" priority="300" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="295" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="208" priority="301" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="296" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="207" priority="302" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 F15 R15 V15">
-    <cfRule type="containsText" dxfId="191" priority="291" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="206" priority="297" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="292" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="205" priority="298" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="293" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="204" priority="299" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17 F17 R17 V17">
-    <cfRule type="containsText" dxfId="188" priority="288" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="203" priority="294" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="289" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="202" priority="295" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="290" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="201" priority="296" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23 F23 R23 V23">
-    <cfRule type="containsText" dxfId="185" priority="282" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="200" priority="288" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="283" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="199" priority="289" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="284" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="198" priority="290" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25 F25 R25 V25">
-    <cfRule type="containsText" dxfId="182" priority="279" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="197" priority="285" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="280" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="196" priority="286" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="281" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="195" priority="287" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27 F27 R27 V27">
-    <cfRule type="containsText" dxfId="179" priority="276" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="194" priority="282" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="277" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="193" priority="283" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="278" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="192" priority="284" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29 F29 R29 V29">
-    <cfRule type="containsText" dxfId="176" priority="273" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="191" priority="279" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="274" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="190" priority="280" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="275" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="189" priority="281" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33 F33 R33 V33">
-    <cfRule type="containsText" dxfId="173" priority="270" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="188" priority="276" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="271" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="187" priority="277" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="272" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="186" priority="278" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35 F35 R35 V35">
-    <cfRule type="containsText" dxfId="170" priority="267" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="185" priority="273" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="268" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="184" priority="274" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="269" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="183" priority="275" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37 F37 R37 V37">
-    <cfRule type="containsText" dxfId="167" priority="264" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="182" priority="270" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="265" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="181" priority="271" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="266" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="180" priority="272" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39 F39 R39 V39">
-    <cfRule type="containsText" dxfId="164" priority="261" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="179" priority="267" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="262" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="178" priority="268" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="263" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="177" priority="269" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41 F41 R41 V41">
-    <cfRule type="containsText" dxfId="161" priority="258" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="176" priority="264" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="259" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="175" priority="265" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="260" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="174" priority="266" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47 F47 R47 V47">
-    <cfRule type="containsText" dxfId="158" priority="255" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="173" priority="261" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="256" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="172" priority="262" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="257" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="171" priority="263" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49 F49 R49 V49">
-    <cfRule type="containsText" dxfId="155" priority="252" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="170" priority="258" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="253" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="169" priority="259" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="254" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="168" priority="260" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R51 V51">
-    <cfRule type="containsText" dxfId="152" priority="249" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="167" priority="255" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="250" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="166" priority="256" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="251" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="165" priority="257" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53 R53 V53">
-    <cfRule type="containsText" dxfId="149" priority="246" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="164" priority="252" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="247" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="163" priority="253" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="248" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="162" priority="254" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55 F55 R55 V55">
-    <cfRule type="containsText" dxfId="146" priority="243" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="161" priority="249" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="244" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="160" priority="250" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="245" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="159" priority="251" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57 F57 R57 V57">
-    <cfRule type="containsText" dxfId="143" priority="240" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="158" priority="246" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="241" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="157" priority="247" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="242" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="156" priority="248" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="containsText" dxfId="140" priority="237" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="155" priority="243" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="238" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="154" priority="244" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="239" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="153" priority="245" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45">
-    <cfRule type="containsText" dxfId="137" priority="234" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="152" priority="240" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="235" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="151" priority="241" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="236" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="150" priority="242" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R45">
-    <cfRule type="containsText" dxfId="134" priority="219" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="149" priority="225" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="220" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="148" priority="226" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="221" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="147" priority="227" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R43">
-    <cfRule type="containsText" dxfId="131" priority="216" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="146" priority="222" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="217" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="145" priority="223" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="218" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="144" priority="224" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V43">
-    <cfRule type="containsText" dxfId="128" priority="213" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="143" priority="219" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",V43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="214" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="142" priority="220" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",V43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="215" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="141" priority="221" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",V43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V45">
-    <cfRule type="containsText" dxfId="125" priority="210" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="140" priority="216" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",V45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="211" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="139" priority="217" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",V45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="212" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="138" priority="218" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",V45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="containsText" dxfId="122" priority="207" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="137" priority="213" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="208" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="136" priority="214" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="209" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="135" priority="215" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R31">
-    <cfRule type="containsText" dxfId="119" priority="198" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="134" priority="204" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="199" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="133" priority="205" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="200" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="132" priority="206" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V31">
-    <cfRule type="containsText" dxfId="116" priority="195" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="131" priority="201" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",V31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="196" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="130" priority="202" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",V31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="197" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="129" priority="203" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",V31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="113" priority="192" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="128" priority="198" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="193" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="127" priority="199" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="194" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="126" priority="200" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19">
-    <cfRule type="containsText" dxfId="110" priority="183" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="125" priority="189" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="184" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="124" priority="190" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="185" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="123" priority="191" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V19">
-    <cfRule type="containsText" dxfId="107" priority="180" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="122" priority="186" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",V19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="181" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="121" priority="187" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",V19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="182" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="120" priority="188" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",V19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="104" priority="177" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="119" priority="183" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="178" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="118" priority="184" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="179" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="117" priority="185" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="containsText" dxfId="101" priority="174" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="116" priority="180" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="175" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="115" priority="181" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="176" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="114" priority="182" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="containsText" dxfId="98" priority="171" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="113" priority="177" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="172" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="112" priority="178" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="173" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="111" priority="179" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="95" priority="168" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="110" priority="174" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="169" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="109" priority="175" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="170" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="108" priority="176" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="containsText" dxfId="92" priority="165" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="107" priority="171" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="166" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="106" priority="172" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="167" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="105" priority="173" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:Y62">
-    <cfRule type="containsText" dxfId="89" priority="162" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="104" priority="168" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="163" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="103" priority="169" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="164" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="102" priority="170" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="containsText" dxfId="86" priority="159" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="101" priority="165" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="160" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="100" priority="166" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="161" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="99" priority="167" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="containsText" dxfId="83" priority="156" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="98" priority="162" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="157" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="97" priority="163" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="158" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="96" priority="164" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z63:Z64">
-    <cfRule type="containsText" dxfId="80" priority="154" operator="containsText" text="INCOMPLETE">
+    <cfRule type="containsText" dxfId="95" priority="160" operator="containsText" text="INCOMPLETE">
       <formula>NOT(ISERROR(SEARCH("INCOMPLETE",Z63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="155" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="94" priority="161" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",Z63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="containsText" dxfId="78" priority="151" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="93" priority="157" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="152" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="92" priority="158" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="153" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="91" priority="159" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q16 N14:Q14 N12:Q12 N10:Q10">
-    <cfRule type="containsText" dxfId="75" priority="139" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="90" priority="145" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",N10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="140" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="89" priority="146" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",N10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="141" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="88" priority="147" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",N10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42:Q42 N40:Q40 N38:Q38 N36:Q36 N34:Q34 N32:Q32 N30:Q30 N28:Q28 N26:Q26 N24:Q24 N22:Q22 N20:Q20 N18:Q18">
-    <cfRule type="containsText" dxfId="72" priority="136" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="87" priority="142" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="137" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="86" priority="143" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="138" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="85" priority="144" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",N18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56:Q56 N54:Q54 N52:Q52 N50:Q50 N48:Q48 N46:Q46 N44:Q44">
-    <cfRule type="containsText" dxfId="69" priority="133" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="84" priority="139" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",N44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="134" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="83" priority="140" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",N44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="135" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="82" priority="141" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",N44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="containsText" dxfId="78" priority="67" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="77" priority="68" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="containsText" dxfId="75" priority="64" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="65" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="66" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15">
+    <cfRule type="containsText" dxfId="72" priority="61" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="71" priority="62" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J17">
+    <cfRule type="containsText" dxfId="69" priority="58" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="59" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J19">
+    <cfRule type="containsText" dxfId="66" priority="55" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="56" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23">
+    <cfRule type="containsText" dxfId="63" priority="52" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="53" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J25">
+    <cfRule type="containsText" dxfId="60" priority="49" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="50" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J25)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J27">
+    <cfRule type="containsText" dxfId="57" priority="46" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="47" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J27)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="55" priority="48" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="containsText" dxfId="54" priority="43" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="44" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J29)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="45" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31">
+    <cfRule type="containsText" dxfId="51" priority="40" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="41" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J31)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="42" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J35">
+    <cfRule type="containsText" dxfId="48" priority="37" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="38" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="39" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J51">
+    <cfRule type="containsText" dxfId="45" priority="34" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="35" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="36" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J49">
+    <cfRule type="containsText" dxfId="42" priority="31" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="32" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="33" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47">
+    <cfRule type="containsText" dxfId="39" priority="28" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="29" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="30" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45">
+    <cfRule type="containsText" dxfId="36" priority="25" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J45)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="26" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J45)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="27" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J43">
+    <cfRule type="containsText" dxfId="33" priority="22" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="23" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J43)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41">
+    <cfRule type="containsText" dxfId="30" priority="19" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="20" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="21" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J39">
+    <cfRule type="containsText" dxfId="27" priority="16" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="17" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J39)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="18" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J39)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21">
+    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37">
+    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J37)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J53">
+    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",J53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",J53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",J53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="┄">
+      <formula>NOT(ISERROR(SEARCH("┄",F21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="✗">
+      <formula>NOT(ISERROR(SEARCH("✗",F21)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="✔">
+      <formula>NOT(ISERROR(SEARCH("✔",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33">
-    <cfRule type="containsText" dxfId="66" priority="100" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="101" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="102" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="containsText" dxfId="63" priority="61" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="62" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="63" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
-    <cfRule type="containsText" dxfId="60" priority="58" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="59" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="60" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J15">
-    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J17">
-    <cfRule type="containsText" dxfId="54" priority="52" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="53" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="54" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J19">
-    <cfRule type="containsText" dxfId="51" priority="49" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J23">
-    <cfRule type="containsText" dxfId="48" priority="46" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J25">
-    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J27">
-    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J29">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J31">
-    <cfRule type="containsText" dxfId="36" priority="34" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
-    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J51">
-    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J51)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J49">
-    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J49)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J47">
-    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J45">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J43">
-    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J41">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J39">
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J21">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J37">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J53">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="┄">
-      <formula>NOT(ISERROR(SEARCH("┄",J53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="✗">
-      <formula>NOT(ISERROR(SEARCH("✗",J53)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="✔">
-      <formula>NOT(ISERROR(SEARCH("✔",J53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11107,7 +11287,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="317" id="{9BB05CC5-38CF-764F-A36E-A7D2A3718881}">
+          <x14:cfRule type="expression" priority="323" id="{9BB05CC5-38CF-764F-A36E-A7D2A3718881}">
             <xm:f>Drop_Down!$A$1</xm:f>
             <x14:dxf>
               <font>
@@ -11130,7 +11310,7 @@
           <x14:formula1>
             <xm:f>Drop_Down!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B50:Q50 B62:Y62 B10:Q10 B12:Q12 B44:Q44 B14:Q14 B16:Q16 B20:Q20 B18:Q18 B24:Q24 B26:Q26 B48:Q48 B46:Q46 B54:Q54 B40:Q40 B42:Q42 B38:Q38 B28:Q28 B34:Q34 B56:Q56 B30:Q30 B32:Q32 B22:Q22 B36:Q36 B52:Q52</xm:sqref>
+          <xm:sqref>B50:Q50 B62:Y62 B10:Q10 B12:Q12 B44:Q44 B14:Q14 B16:Q16 B20:Q20 B18:Q18 B24:Q24 B26:Q26 B48:Q48 B46:Q46 B54:Q54 B40:Q40 B42:Q42 B38:Q38 B28:Q28 B34:Q34 B56:Q56 B30:Q30 B52:Q52 B22:Q22 B36:Q36 B32:Q32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -11254,58 +11434,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="121" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
       <c r="M1" s="40"/>
       <c r="N1" s="40"/>
       <c r="O1" s="40"/>
       <c r="P1" s="40"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="119"/>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
+      <c r="A2" s="121"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
       <c r="M2" s="40"/>
-      <c r="N2" s="118" t="s">
+      <c r="N2" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="120"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="119"/>
-      <c r="B3" s="119"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
+      <c r="A3" s="121"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
       <c r="M3" s="41"/>
       <c r="N3" s="40" t="s">
         <v>61</v>
@@ -11318,18 +11498,18 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1">
-      <c r="A4" s="119"/>
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="119"/>
-      <c r="L4" s="119"/>
+      <c r="A4" s="121"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
       <c r="M4" s="1"/>
       <c r="N4" s="40" t="s">
         <v>62</v>
@@ -11711,11 +11891,11 @@
         <v>1488</v>
       </c>
       <c r="M12" s="41"/>
-      <c r="N12" s="118" t="s">
+      <c r="N12" s="120" t="s">
         <v>70</v>
       </c>
-      <c r="O12" s="118"/>
-      <c r="P12" s="118"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">

</xml_diff>

<commit_message>
related-posts and related-posts__item working Needs to be refactored thoroughly and tested
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="146">
+  <cellStyleXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -676,6 +676,10 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1171,7 +1175,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="146">
+  <cellStyles count="150">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1244,6 +1248,8 @@
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1316,100 +1322,12 @@
     <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="7" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="224">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="269">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3529,6 +3447,546 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3891,8 +4349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32:M32"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AA55" sqref="AA55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4406,7 +4864,7 @@
         <v>37</v>
       </c>
       <c r="Z10" s="98" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA10" s="36"/>
       <c r="AB10" s="36"/>
@@ -4548,7 +5006,7 @@
         <v>37</v>
       </c>
       <c r="Z12" s="61" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA12" s="36"/>
       <c r="AB12" s="36"/>
@@ -4690,7 +5148,7 @@
         <v>37</v>
       </c>
       <c r="Z14" s="61" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA14" s="54"/>
       <c r="AB14" s="36"/>
@@ -4832,7 +5290,7 @@
         <v>37</v>
       </c>
       <c r="Z16" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA16" s="36"/>
       <c r="AB16" s="36"/>
@@ -4974,7 +5432,7 @@
         <v>37</v>
       </c>
       <c r="Z18" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA18" s="36"/>
       <c r="AB18" s="36"/>
@@ -5116,7 +5574,7 @@
         <v>37</v>
       </c>
       <c r="Z20" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA20" s="36"/>
       <c r="AB20" s="36"/>
@@ -5258,7 +5716,7 @@
         <v>37</v>
       </c>
       <c r="Z22" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA22" s="36"/>
       <c r="AB22" s="36"/>
@@ -5400,7 +5858,7 @@
         <v>37</v>
       </c>
       <c r="Z24" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA24" s="36"/>
       <c r="AB24" s="36"/>
@@ -5542,7 +6000,7 @@
         <v>37</v>
       </c>
       <c r="Z26" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA26" s="36"/>
       <c r="AB26" s="36"/>
@@ -5684,7 +6142,7 @@
         <v>37</v>
       </c>
       <c r="Z28" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA28" s="36"/>
       <c r="AB28" s="36"/>
@@ -5826,7 +6284,7 @@
         <v>37</v>
       </c>
       <c r="Z30" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA30" s="36"/>
       <c r="AB30" s="36"/>
@@ -5968,7 +6426,7 @@
         <v>37</v>
       </c>
       <c r="Z32" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA32" s="36"/>
       <c r="AB32" s="36"/>
@@ -6110,7 +6568,7 @@
         <v>37</v>
       </c>
       <c r="Z34" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA34" s="36"/>
       <c r="AB34" s="36"/>
@@ -6252,7 +6710,7 @@
         <v>37</v>
       </c>
       <c r="Z36" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA36" s="36"/>
       <c r="AB36" s="36"/>
@@ -6394,7 +6852,7 @@
         <v>37</v>
       </c>
       <c r="Z38" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA38" s="36"/>
       <c r="AB38" s="36"/>
@@ -6536,7 +6994,7 @@
         <v>37</v>
       </c>
       <c r="Z40" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA40" s="36"/>
       <c r="AB40" s="36"/>
@@ -6678,7 +7136,7 @@
         <v>37</v>
       </c>
       <c r="Z42" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA42" s="36"/>
       <c r="AB42" s="36"/>
@@ -6820,7 +7278,7 @@
         <v>37</v>
       </c>
       <c r="Z44" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA44" s="36"/>
       <c r="AB44" s="36"/>
@@ -6962,7 +7420,7 @@
         <v>37</v>
       </c>
       <c r="Z46" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA46" s="36"/>
       <c r="AB46" s="36"/>
@@ -7104,7 +7562,7 @@
         <v>37</v>
       </c>
       <c r="Z48" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA48" s="36"/>
       <c r="AB48" s="36"/>
@@ -7246,7 +7704,7 @@
         <v>37</v>
       </c>
       <c r="Z50" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA50" s="36"/>
       <c r="AB50" s="36"/>
@@ -7388,7 +7846,7 @@
         <v>37</v>
       </c>
       <c r="Z52" s="61" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="AA52" s="36"/>
       <c r="AB52" s="36"/>
@@ -7530,7 +7988,7 @@
         <v>37</v>
       </c>
       <c r="Z54" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA54" s="36"/>
       <c r="AB54" s="36"/>
@@ -7672,7 +8130,7 @@
         <v>37</v>
       </c>
       <c r="Z56" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA56" s="36"/>
       <c r="AB56" s="36"/>
@@ -7724,7 +8182,7 @@
       <c r="W57" s="105"/>
       <c r="X57" s="105"/>
       <c r="Y57" s="106"/>
-      <c r="Z57" s="61"/>
+      <c r="Z57" s="64"/>
       <c r="AA57" s="53"/>
       <c r="AB57" s="53"/>
       <c r="AC57" s="53"/>
@@ -7754,7 +8212,7 @@
       <c r="H58" s="85"/>
       <c r="I58" s="86"/>
       <c r="J58" s="84" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="K58" s="85"/>
       <c r="L58" s="85"/>
@@ -7848,7 +8306,7 @@
       <c r="H60" s="60"/>
       <c r="I60" s="61"/>
       <c r="J60" s="59" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K60" s="60"/>
       <c r="L60" s="60"/>
@@ -10505,779 +10963,779 @@
     <mergeCell ref="V63:Y64"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:M10 B11 F11 R11 V11 B12:M12 B20:M20 B24:M24 B26:M26 B14:M14 B16:M16 B18:M18 B22:M22 B28:M28 B30:M30 B34:M34 B38:M38 B40:M40 B42:M42 B44:M44 B46:M46 B48:M48 B50:M50 B54:M54 B56:M56 B36:M36 B52:M52 B32:M32">
-    <cfRule type="containsText" dxfId="223" priority="320" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="214" priority="320" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="321" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="213" priority="321" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="322" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="212" priority="322" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60:Y62">
-    <cfRule type="containsText" dxfId="220" priority="316" operator="containsText" text="IN-PROGRESS">
+    <cfRule type="containsText" dxfId="211" priority="316" operator="containsText" text="IN-PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN-PROGRESS",B60)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="219" priority="317" operator="containsText" text="COMPLETED">
+    <cfRule type="containsText" dxfId="210" priority="317" operator="containsText" text="COMPLETED">
       <formula>NOT(ISERROR(SEARCH("COMPLETED",B60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:Y64 Z62">
-    <cfRule type="containsText" dxfId="218" priority="310" operator="containsText" text="INCOMPLETE">
+    <cfRule type="containsText" dxfId="209" priority="310" operator="containsText" text="INCOMPLETE">
       <formula>NOT(ISERROR(SEARCH("INCOMPLETE",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="217" priority="311" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="208" priority="311" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z60:Z61">
-    <cfRule type="containsText" dxfId="216" priority="309" operator="containsText" text="IN-PROGRESS">
+    <cfRule type="containsText" dxfId="207" priority="309" operator="containsText" text="IN-PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN-PROGRESS",Z60)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z10:Z57 B58:Z59">
-    <cfRule type="containsText" dxfId="215" priority="306" operator="containsText" text="NO">
+  <conditionalFormatting sqref="B58:Z59 Z10:Z57">
+    <cfRule type="containsText" dxfId="206" priority="306" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="307" operator="containsText" text="PARTIALLY">
+    <cfRule type="containsText" dxfId="205" priority="307" operator="containsText" text="PARTIALLY">
       <formula>NOT(ISERROR(SEARCH("PARTIALLY",B10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="213" priority="308" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="204" priority="308" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 R21 V21">
-    <cfRule type="containsText" dxfId="212" priority="291" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="203" priority="291" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="211" priority="292" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="202" priority="292" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="293" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="201" priority="293" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13 R13 V13">
-    <cfRule type="containsText" dxfId="209" priority="300" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="200" priority="300" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="208" priority="301" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="199" priority="301" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="207" priority="302" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="198" priority="302" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 F15 R15 V15">
-    <cfRule type="containsText" dxfId="206" priority="297" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="197" priority="297" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="205" priority="298" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="196" priority="298" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="204" priority="299" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="195" priority="299" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17 F17 R17 V17">
-    <cfRule type="containsText" dxfId="203" priority="294" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="194" priority="294" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="295" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="193" priority="295" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="296" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="192" priority="296" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23 F23 R23 V23">
-    <cfRule type="containsText" dxfId="200" priority="288" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="191" priority="288" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="289" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="190" priority="289" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="290" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="189" priority="290" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25 F25 R25 V25">
-    <cfRule type="containsText" dxfId="197" priority="285" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="188" priority="285" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="286" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="187" priority="286" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="287" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="186" priority="287" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27 F27 R27 V27">
-    <cfRule type="containsText" dxfId="194" priority="282" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="185" priority="282" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="283" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="184" priority="283" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="284" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="183" priority="284" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29 F29 R29 V29">
-    <cfRule type="containsText" dxfId="191" priority="279" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="182" priority="279" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="280" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="181" priority="280" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="189" priority="281" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="180" priority="281" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33 F33 R33 V33">
-    <cfRule type="containsText" dxfId="188" priority="276" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="179" priority="276" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="277" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="178" priority="277" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="278" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="177" priority="278" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35 F35 R35 V35">
-    <cfRule type="containsText" dxfId="185" priority="273" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="176" priority="273" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="274" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="175" priority="274" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="275" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="174" priority="275" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37 F37 R37 V37">
-    <cfRule type="containsText" dxfId="182" priority="270" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="173" priority="270" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="271" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="172" priority="271" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="272" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="171" priority="272" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39 F39 R39 V39">
-    <cfRule type="containsText" dxfId="179" priority="267" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="170" priority="267" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="178" priority="268" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="169" priority="268" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="269" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="168" priority="269" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41 F41 R41 V41">
-    <cfRule type="containsText" dxfId="176" priority="264" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="167" priority="264" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="265" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="166" priority="265" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="174" priority="266" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="165" priority="266" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47 F47 R47 V47">
-    <cfRule type="containsText" dxfId="173" priority="261" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="164" priority="261" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="172" priority="262" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="163" priority="262" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="263" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="162" priority="263" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49 F49 R49 V49">
-    <cfRule type="containsText" dxfId="170" priority="258" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="161" priority="258" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="169" priority="259" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="160" priority="259" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="168" priority="260" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="159" priority="260" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R51 V51">
-    <cfRule type="containsText" dxfId="167" priority="255" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="158" priority="255" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="256" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="157" priority="256" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="257" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="156" priority="257" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53 R53 V53">
-    <cfRule type="containsText" dxfId="164" priority="252" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="155" priority="252" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="253" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="154" priority="253" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="254" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="153" priority="254" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55 F55 R55 V55">
-    <cfRule type="containsText" dxfId="161" priority="249" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="152" priority="249" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="250" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="151" priority="250" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="251" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="150" priority="251" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57 F57 R57 V57">
-    <cfRule type="containsText" dxfId="158" priority="246" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="149" priority="246" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="247" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="148" priority="247" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="248" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="147" priority="248" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43">
-    <cfRule type="containsText" dxfId="155" priority="243" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="146" priority="243" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="244" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="145" priority="244" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="245" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="144" priority="245" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45">
-    <cfRule type="containsText" dxfId="152" priority="240" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="143" priority="240" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="241" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="142" priority="241" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="242" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="141" priority="242" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R45">
-    <cfRule type="containsText" dxfId="149" priority="225" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="140" priority="225" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="226" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="139" priority="226" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="227" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="138" priority="227" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R43">
-    <cfRule type="containsText" dxfId="146" priority="222" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="137" priority="222" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="223" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="136" priority="223" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="224" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="135" priority="224" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V43">
-    <cfRule type="containsText" dxfId="143" priority="219" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="134" priority="219" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",V43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="220" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="133" priority="220" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",V43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="221" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="132" priority="221" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",V43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V45">
-    <cfRule type="containsText" dxfId="140" priority="216" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="131" priority="216" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",V45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="217" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="130" priority="217" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",V45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="218" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="129" priority="218" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",V45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31">
-    <cfRule type="containsText" dxfId="137" priority="213" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="128" priority="213" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="214" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="127" priority="214" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="215" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="126" priority="215" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R31">
-    <cfRule type="containsText" dxfId="134" priority="204" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="125" priority="204" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="205" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="124" priority="205" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="206" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="123" priority="206" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V31">
-    <cfRule type="containsText" dxfId="131" priority="201" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="122" priority="201" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",V31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="202" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="121" priority="202" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",V31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="203" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="120" priority="203" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",V31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="128" priority="198" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="119" priority="198" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="199" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="118" priority="199" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="200" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="117" priority="200" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19">
-    <cfRule type="containsText" dxfId="125" priority="189" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="116" priority="189" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",R19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="190" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="115" priority="190" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",R19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="191" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="114" priority="191" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",R19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V19">
-    <cfRule type="containsText" dxfId="122" priority="186" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="113" priority="186" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",V19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="187" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="112" priority="187" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",V19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="188" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="111" priority="188" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",V19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="119" priority="183" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="110" priority="183" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="184" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="109" priority="184" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="185" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="108" priority="185" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="containsText" dxfId="116" priority="180" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="107" priority="180" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="181" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="106" priority="181" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="182" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="105" priority="182" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="containsText" dxfId="113" priority="177" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="104" priority="177" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="178" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="103" priority="178" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="179" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="102" priority="179" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="containsText" dxfId="110" priority="174" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="101" priority="174" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="175" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="100" priority="175" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="176" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="99" priority="176" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="containsText" dxfId="107" priority="171" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="98" priority="171" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="172" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="97" priority="172" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="173" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="96" priority="173" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:Y62">
-    <cfRule type="containsText" dxfId="104" priority="168" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="95" priority="168" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="169" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="94" priority="169" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",B62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="170" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="93" priority="170" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",B62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="containsText" dxfId="101" priority="165" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="92" priority="165" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="166" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="91" priority="166" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="167" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="90" priority="167" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="containsText" dxfId="98" priority="162" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="89" priority="162" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="163" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="88" priority="163" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="164" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="87" priority="164" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z63:Z64">
-    <cfRule type="containsText" dxfId="95" priority="160" operator="containsText" text="INCOMPLETE">
+    <cfRule type="containsText" dxfId="86" priority="160" operator="containsText" text="INCOMPLETE">
       <formula>NOT(ISERROR(SEARCH("INCOMPLETE",Z63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="161" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="85" priority="161" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",Z63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="containsText" dxfId="93" priority="157" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="84" priority="157" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="158" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="83" priority="158" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="159" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="82" priority="159" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q16 N14:Q14 N12:Q12 N10:Q10">
-    <cfRule type="containsText" dxfId="90" priority="145" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="81" priority="145" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",N10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="146" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="80" priority="146" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",N10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="147" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="79" priority="147" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",N10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N42:Q42 N40:Q40 N38:Q38 N36:Q36 N34:Q34 N32:Q32 N30:Q30 N28:Q28 N26:Q26 N24:Q24 N22:Q22 N20:Q20 N18:Q18">
-    <cfRule type="containsText" dxfId="87" priority="142" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="78" priority="142" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="143" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="77" priority="143" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="144" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="76" priority="144" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",N18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56:Q56 N54:Q54 N52:Q52 N50:Q50 N48:Q48 N46:Q46 N44:Q44">
-    <cfRule type="containsText" dxfId="84" priority="139" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="75" priority="139" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",N44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="140" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="74" priority="140" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",N44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="141" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="73" priority="141" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",N44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="containsText" dxfId="78" priority="67" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="69" priority="67" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="68" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="68" priority="68" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="69" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="67" priority="69" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="containsText" dxfId="75" priority="64" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="66" priority="64" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="65" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="65" priority="65" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="66" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="64" priority="66" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="containsText" dxfId="72" priority="61" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="63" priority="61" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="62" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="62" priority="62" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="63" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="61" priority="63" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="containsText" dxfId="69" priority="58" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="60" priority="58" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="59" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="59" priority="59" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="58" priority="60" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19">
-    <cfRule type="containsText" dxfId="66" priority="55" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="56" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="containsText" dxfId="63" priority="52" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="54" priority="52" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="53" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="53" priority="53" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="52" priority="54" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="containsText" dxfId="60" priority="49" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="51" priority="49" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="50" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="49" priority="51" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27">
-    <cfRule type="containsText" dxfId="57" priority="46" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="48" priority="46" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="47" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="47" priority="47" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="48" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="46" priority="48" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="containsText" dxfId="54" priority="43" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="44" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="45" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="containsText" dxfId="51" priority="40" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="41" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="42" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="containsText" dxfId="48" priority="37" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="38" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="39" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51">
-    <cfRule type="containsText" dxfId="45" priority="34" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="36" priority="34" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="35" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="36" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49">
-    <cfRule type="containsText" dxfId="42" priority="31" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="32" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="33" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47">
-    <cfRule type="containsText" dxfId="39" priority="28" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="29" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="30" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45">
-    <cfRule type="containsText" dxfId="36" priority="25" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="26" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="27" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43">
-    <cfRule type="containsText" dxfId="33" priority="22" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="23" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41">
-    <cfRule type="containsText" dxfId="30" priority="19" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="20" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="21" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39">
-    <cfRule type="containsText" dxfId="27" priority="16" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="17" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="18" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21">
-    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37">
-    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J53">
-    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="┄">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="┄">
       <formula>NOT(ISERROR(SEARCH("┄",J33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="✗">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="✗">
       <formula>NOT(ISERROR(SEARCH("✗",J33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="✔">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="✔">
       <formula>NOT(ISERROR(SEARCH("✔",J33)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11316,7 +11774,7 @@
           <x14:formula1>
             <xm:f>Drop_Down!$A$5:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>Z10 Z12 Z14 B58:Z59 Z56 Z54 Z52 Z50 Z48 Z46 Z44 Z42 Z40 Z38 Z36 Z34 Z32 Z30 Z28 Z26 Z24 Z22 Z20 Z16 Z18</xm:sqref>
+          <xm:sqref>Z10 Z12 Z14 B58:Z59 Z54 Z52 Z50 Z48 Z46 Z44 Z42 Z40 Z38 Z36 Z34 Z32 Z30 Z28 Z18 Z26 Z24 Z22 Z20 Z16 Z56</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -11423,8 +11881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11584,29 +12042,29 @@
       <c r="D6" s="30">
         <v>448</v>
       </c>
-      <c r="E6" s="37">
-        <v>41.75</v>
-      </c>
-      <c r="F6" s="38">
-        <v>668</v>
+      <c r="E6" s="42">
+        <v>41.6875</v>
+      </c>
+      <c r="F6" s="43">
+        <v>667</v>
       </c>
       <c r="G6" s="29">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" s="28">
-        <v>912</v>
+        <v>896</v>
       </c>
       <c r="I6" s="29">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J6" s="28">
-        <v>1168</v>
+        <v>1152</v>
       </c>
       <c r="K6" s="30">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L6" s="30">
-        <v>1392</v>
+        <v>1376</v>
       </c>
       <c r="M6" s="41"/>
       <c r="N6" s="40" t="s">
@@ -11632,29 +12090,29 @@
       <c r="D7" s="30">
         <v>464</v>
       </c>
-      <c r="E7" s="29">
-        <v>42</v>
-      </c>
-      <c r="F7" s="30">
-        <v>672</v>
+      <c r="E7" s="37">
+        <v>41.75</v>
+      </c>
+      <c r="F7" s="38">
+        <v>668</v>
       </c>
       <c r="G7" s="29">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="28">
-        <v>928</v>
+        <v>912</v>
       </c>
       <c r="I7" s="29">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J7" s="28">
-        <v>1184</v>
+        <v>1168</v>
       </c>
       <c r="K7" s="30">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L7" s="30">
-        <v>1408</v>
+        <v>1392</v>
       </c>
       <c r="M7" s="41"/>
       <c r="N7" s="40" t="s">
@@ -11681,28 +12139,28 @@
         <v>480</v>
       </c>
       <c r="E8" s="29">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="30">
-        <v>688</v>
+        <v>672</v>
       </c>
       <c r="G8" s="29">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" s="28">
-        <v>944</v>
-      </c>
-      <c r="I8" s="23">
-        <v>75</v>
-      </c>
-      <c r="J8" s="24">
-        <v>1200</v>
+        <v>928</v>
+      </c>
+      <c r="I8" s="29">
+        <v>74</v>
+      </c>
+      <c r="J8" s="28">
+        <v>1184</v>
       </c>
       <c r="K8" s="30">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L8" s="30">
-        <v>1424</v>
+        <v>1408</v>
       </c>
       <c r="M8" s="41"/>
       <c r="N8" s="40" t="s">
@@ -11729,28 +12187,28 @@
         <v>496</v>
       </c>
       <c r="E9" s="29">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="30">
-        <v>704</v>
+        <v>688</v>
       </c>
       <c r="G9" s="29">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="28">
-        <v>960</v>
-      </c>
-      <c r="I9" s="29">
-        <v>76</v>
-      </c>
-      <c r="J9" s="28">
-        <v>1216</v>
+        <v>944</v>
+      </c>
+      <c r="I9" s="23">
+        <v>75</v>
+      </c>
+      <c r="J9" s="24">
+        <v>1200</v>
       </c>
       <c r="K9" s="30">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" s="30">
-        <v>1440</v>
+        <v>1424</v>
       </c>
       <c r="M9" s="41"/>
       <c r="N9" s="40" t="s">
@@ -11771,34 +12229,34 @@
         <v>304</v>
       </c>
       <c r="C10" s="25">
-        <v>32</v>
+        <v>31.25</v>
       </c>
       <c r="D10" s="27">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="E10" s="29">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="30">
-        <v>720</v>
+        <v>704</v>
       </c>
       <c r="G10" s="29">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H10" s="28">
-        <v>976</v>
+        <v>960</v>
       </c>
       <c r="I10" s="29">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" s="28">
-        <v>1232</v>
+        <v>1216</v>
       </c>
       <c r="K10" s="30">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L10" s="30">
-        <v>1456</v>
+        <v>1440</v>
       </c>
       <c r="M10" s="40"/>
       <c r="N10" s="40" t="s">
@@ -11818,35 +12276,35 @@
       <c r="B11" s="38">
         <v>320</v>
       </c>
-      <c r="C11" s="29">
-        <v>33</v>
-      </c>
-      <c r="D11" s="30">
-        <v>528</v>
-      </c>
-      <c r="E11" s="37">
-        <v>46</v>
-      </c>
-      <c r="F11" s="38">
-        <v>736</v>
-      </c>
-      <c r="G11" s="25">
-        <v>62</v>
-      </c>
-      <c r="H11" s="26">
-        <v>992</v>
+      <c r="C11" s="25">
+        <v>32</v>
+      </c>
+      <c r="D11" s="27">
+        <v>512</v>
+      </c>
+      <c r="E11" s="29">
+        <v>45</v>
+      </c>
+      <c r="F11" s="30">
+        <v>720</v>
+      </c>
+      <c r="G11" s="29">
+        <v>61</v>
+      </c>
+      <c r="H11" s="28">
+        <v>976</v>
       </c>
       <c r="I11" s="29">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J11" s="28">
-        <v>1248</v>
+        <v>1232</v>
       </c>
       <c r="K11" s="30">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L11" s="30">
-        <v>1472</v>
+        <v>1456</v>
       </c>
       <c r="M11" s="40"/>
       <c r="N11" s="41"/>
@@ -11860,35 +12318,35 @@
       <c r="B12" s="28">
         <v>336</v>
       </c>
-      <c r="C12" s="25">
-        <v>34</v>
-      </c>
-      <c r="D12" s="27">
-        <v>544</v>
-      </c>
-      <c r="E12" s="29">
-        <v>47</v>
-      </c>
-      <c r="F12" s="28">
-        <v>752</v>
-      </c>
-      <c r="G12" s="29">
-        <v>63</v>
-      </c>
-      <c r="H12" s="28">
-        <v>1008</v>
-      </c>
-      <c r="I12" s="30">
-        <v>79</v>
+      <c r="C12" s="29">
+        <v>33</v>
+      </c>
+      <c r="D12" s="30">
+        <v>528</v>
+      </c>
+      <c r="E12" s="37">
+        <v>46</v>
+      </c>
+      <c r="F12" s="38">
+        <v>736</v>
+      </c>
+      <c r="G12" s="25">
+        <v>62</v>
+      </c>
+      <c r="H12" s="26">
+        <v>992</v>
+      </c>
+      <c r="I12" s="29">
+        <v>78</v>
       </c>
       <c r="J12" s="28">
-        <v>1264</v>
+        <v>1248</v>
       </c>
       <c r="K12" s="30">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L12" s="30">
-        <v>1488</v>
+        <v>1472</v>
       </c>
       <c r="M12" s="41"/>
       <c r="N12" s="120" t="s">
@@ -11905,35 +12363,35 @@
       <c r="B13" s="30">
         <v>352</v>
       </c>
-      <c r="C13" s="29">
-        <v>35</v>
-      </c>
-      <c r="D13" s="30">
-        <v>560</v>
-      </c>
-      <c r="E13" s="25">
-        <v>48</v>
-      </c>
-      <c r="F13" s="26">
-        <v>768</v>
-      </c>
-      <c r="G13" s="25">
-        <v>64</v>
-      </c>
-      <c r="H13" s="26">
-        <v>1024</v>
+      <c r="C13" s="25">
+        <v>34</v>
+      </c>
+      <c r="D13" s="27">
+        <v>544</v>
+      </c>
+      <c r="E13" s="29">
+        <v>47</v>
+      </c>
+      <c r="F13" s="28">
+        <v>752</v>
+      </c>
+      <c r="G13" s="29">
+        <v>63</v>
+      </c>
+      <c r="H13" s="28">
+        <v>1008</v>
       </c>
       <c r="I13" s="30">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J13" s="28">
-        <v>1280</v>
+        <v>1264</v>
       </c>
       <c r="K13" s="30">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L13" s="30">
-        <v>1504</v>
+        <v>1488</v>
       </c>
       <c r="M13" s="40"/>
       <c r="N13" s="40" t="s">
@@ -11953,35 +12411,35 @@
       <c r="B14" s="30">
         <v>368</v>
       </c>
-      <c r="C14" s="25">
-        <v>35.5</v>
-      </c>
-      <c r="D14" s="27">
-        <v>568</v>
-      </c>
-      <c r="E14" s="29">
-        <v>49</v>
-      </c>
-      <c r="F14" s="28">
-        <v>784</v>
-      </c>
-      <c r="G14" s="29">
-        <v>65</v>
-      </c>
-      <c r="H14" s="28">
-        <v>1040</v>
+      <c r="C14" s="29">
+        <v>35</v>
+      </c>
+      <c r="D14" s="30">
+        <v>560</v>
+      </c>
+      <c r="E14" s="25">
+        <v>48</v>
+      </c>
+      <c r="F14" s="26">
+        <v>768</v>
+      </c>
+      <c r="G14" s="25">
+        <v>64</v>
+      </c>
+      <c r="H14" s="26">
+        <v>1024</v>
       </c>
       <c r="I14" s="30">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J14" s="28">
-        <v>1296</v>
-      </c>
-      <c r="K14" s="34">
-        <v>95</v>
-      </c>
-      <c r="L14" s="34">
-        <v>1520</v>
+        <v>1280</v>
+      </c>
+      <c r="K14" s="30">
+        <v>94</v>
+      </c>
+      <c r="L14" s="30">
+        <v>1504</v>
       </c>
       <c r="M14" s="40"/>
       <c r="N14" s="40" t="s">
@@ -12001,35 +12459,35 @@
       <c r="B15" s="38">
         <v>375</v>
       </c>
-      <c r="C15" s="29">
-        <v>36</v>
-      </c>
-      <c r="D15" s="30">
-        <v>576</v>
+      <c r="C15" s="25">
+        <v>35.5</v>
+      </c>
+      <c r="D15" s="27">
+        <v>568</v>
       </c>
       <c r="E15" s="29">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="28">
-        <v>800</v>
+        <v>784</v>
       </c>
       <c r="G15" s="29">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H15" s="28">
-        <v>1056</v>
+        <v>1040</v>
       </c>
       <c r="I15" s="30">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J15" s="28">
-        <v>1312</v>
+        <v>1296</v>
       </c>
       <c r="K15" s="34">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L15" s="34">
-        <v>1536</v>
+        <v>1520</v>
       </c>
       <c r="M15" s="40"/>
       <c r="N15" s="40" t="s">
@@ -12050,34 +12508,34 @@
         <v>376</v>
       </c>
       <c r="C16" s="29">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="30">
-        <v>592</v>
+        <v>576</v>
       </c>
       <c r="E16" s="29">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="28">
-        <v>816</v>
+        <v>800</v>
       </c>
       <c r="G16" s="29">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H16" s="28">
-        <v>1072</v>
+        <v>1056</v>
       </c>
       <c r="I16" s="30">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J16" s="28">
-        <v>1328</v>
+        <v>1312</v>
       </c>
       <c r="K16" s="34">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L16" s="34">
-        <v>1552</v>
+        <v>1536</v>
       </c>
       <c r="M16" s="40"/>
       <c r="N16" s="40" t="s">
@@ -12098,34 +12556,34 @@
         <v>384</v>
       </c>
       <c r="C17" s="29">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="30">
-        <v>608</v>
+        <v>592</v>
       </c>
       <c r="E17" s="29">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="28">
-        <v>832</v>
+        <v>816</v>
       </c>
       <c r="G17" s="29">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H17" s="28">
-        <v>1088</v>
+        <v>1072</v>
       </c>
       <c r="I17" s="30">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J17" s="28">
-        <v>1344</v>
+        <v>1328</v>
       </c>
       <c r="K17" s="34">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L17" s="34">
-        <v>1568</v>
+        <v>1552</v>
       </c>
       <c r="M17" s="40"/>
       <c r="N17" s="40" t="s">
@@ -12146,34 +12604,34 @@
         <v>400</v>
       </c>
       <c r="C18" s="29">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="30">
-        <v>624</v>
+        <v>608</v>
       </c>
       <c r="E18" s="29">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" s="28">
-        <v>848</v>
+        <v>832</v>
       </c>
       <c r="G18" s="29">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H18" s="28">
-        <v>1104</v>
+        <v>1088</v>
       </c>
       <c r="I18" s="30">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J18" s="28">
-        <v>1360</v>
+        <v>1344</v>
       </c>
       <c r="K18" s="34">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L18" s="34">
-        <v>1584</v>
+        <v>1568</v>
       </c>
       <c r="M18" s="40"/>
       <c r="N18" s="40" t="s">
@@ -12194,34 +12652,34 @@
         <v>414</v>
       </c>
       <c r="C19" s="29">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="30">
-        <v>640</v>
+        <v>624</v>
       </c>
       <c r="E19" s="29">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" s="28">
-        <v>864</v>
+        <v>848</v>
       </c>
       <c r="G19" s="29">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H19" s="28">
-        <v>1120</v>
-      </c>
-      <c r="I19" s="38">
-        <v>85.375</v>
-      </c>
-      <c r="J19" s="39">
-        <v>1366</v>
+        <v>1104</v>
+      </c>
+      <c r="I19" s="30">
+        <v>85</v>
+      </c>
+      <c r="J19" s="28">
+        <v>1360</v>
       </c>
       <c r="K19" s="34">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L19" s="34">
-        <v>1600</v>
+        <v>1584</v>
       </c>
       <c r="M19" s="40"/>
       <c r="N19" s="40" t="s">
@@ -12242,31 +12700,35 @@
         <v>416</v>
       </c>
       <c r="C20" s="29">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="30">
-        <v>656</v>
+        <v>640</v>
       </c>
       <c r="E20" s="29">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" s="28">
-        <v>880</v>
+        <v>864</v>
       </c>
       <c r="G20" s="29">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H20" s="28">
-        <v>1136</v>
+        <v>1120</v>
       </c>
       <c r="I20" s="38">
-        <v>85.5</v>
+        <v>85.375</v>
       </c>
       <c r="J20" s="39">
-        <v>1368</v>
-      </c>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
+        <v>1366</v>
+      </c>
+      <c r="K20" s="34">
+        <v>100</v>
+      </c>
+      <c r="L20" s="34">
+        <v>1600</v>
+      </c>
       <c r="M20" s="40"/>
       <c r="N20" s="40" t="s">
         <v>68</v>
@@ -12285,29 +12747,29 @@
       <c r="B21" s="28">
         <v>432</v>
       </c>
-      <c r="C21" s="42">
-        <v>41.6875</v>
-      </c>
-      <c r="D21" s="43">
-        <v>667</v>
+      <c r="C21" s="29">
+        <v>41</v>
+      </c>
+      <c r="D21" s="30">
+        <v>656</v>
       </c>
       <c r="E21" s="29">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="28">
-        <v>896</v>
+        <v>880</v>
       </c>
       <c r="G21" s="29">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H21" s="28">
-        <v>1152</v>
-      </c>
-      <c r="I21" s="30">
-        <v>86</v>
-      </c>
-      <c r="J21" s="28">
-        <v>1376</v>
+        <v>1136</v>
+      </c>
+      <c r="I21" s="38">
+        <v>85.5</v>
+      </c>
+      <c r="J21" s="39">
+        <v>1368</v>
       </c>
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>

</xml_diff>